<commit_message>
Added Letter Collection system
</commit_message>
<xml_diff>
--- a/documents/Map/Map.xlsx
+++ b/documents/Map/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athicha/Desktop/JavaGameProject/documents/Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C73564-FBAE-9F44-8947-2D14A9D508F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E4271-A94D-2C44-B0FF-1DD6481D7A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19380" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>EMPTY</t>
   </si>
@@ -79,12 +79,27 @@
   <si>
     <t>WOOD_DOOR</t>
   </si>
+  <si>
+    <t>METAL_WALL</t>
+  </si>
+  <si>
+    <t>WOOD_DOOR_BLOOD</t>
+  </si>
+  <si>
+    <t>LETTER LISTS</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,8 +142,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +236,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -229,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -277,6 +318,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84092400-AD61-BC4A-9F6E-C24F40418E60}">
-  <dimension ref="B2:EF126"/>
+  <dimension ref="B2:ER126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH40" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CP54" sqref="CP54"/>
+    <sheetView tabSelected="1" topLeftCell="BH32" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CF36" sqref="CF36:DU64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1591,7 @@
       <c r="CH32" s="1"/>
       <c r="CQ32" s="1"/>
     </row>
-    <row r="33" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="Y33" s="1"/>
@@ -1553,7 +1609,7 @@
       <c r="CP33" s="1"/>
       <c r="CQ33" s="1"/>
     </row>
-    <row r="34" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
       <c r="I34" s="3"/>
@@ -1569,15 +1625,144 @@
       <c r="AP34" s="1"/>
       <c r="BK34" s="1"/>
     </row>
-    <row r="35" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="Y35" s="1"/>
       <c r="AK35" s="1"/>
       <c r="AP35" s="1"/>
       <c r="BK35" s="1"/>
+      <c r="CF35" s="14">
+        <v>0</v>
+      </c>
+      <c r="CG35" s="14">
+        <v>1</v>
+      </c>
+      <c r="CH35" s="14">
+        <v>2</v>
+      </c>
+      <c r="CI35" s="14">
+        <v>3</v>
+      </c>
+      <c r="CJ35" s="14">
+        <v>4</v>
+      </c>
+      <c r="CK35" s="14">
+        <v>5</v>
+      </c>
+      <c r="CL35" s="14">
+        <v>6</v>
+      </c>
+      <c r="CM35" s="14">
+        <v>7</v>
+      </c>
+      <c r="CN35" s="14">
+        <v>8</v>
+      </c>
+      <c r="CO35" s="14">
+        <v>9</v>
+      </c>
+      <c r="CP35" s="14">
+        <v>10</v>
+      </c>
+      <c r="CQ35" s="14">
+        <v>11</v>
+      </c>
+      <c r="CR35" s="14">
+        <v>12</v>
+      </c>
+      <c r="CS35" s="14">
+        <v>13</v>
+      </c>
+      <c r="CT35" s="14">
+        <v>14</v>
+      </c>
+      <c r="CU35" s="14">
+        <v>15</v>
+      </c>
+      <c r="CV35" s="14">
+        <v>16</v>
+      </c>
+      <c r="CW35" s="14">
+        <v>17</v>
+      </c>
+      <c r="CX35" s="14">
+        <v>18</v>
+      </c>
+      <c r="CY35" s="14">
+        <v>19</v>
+      </c>
+      <c r="CZ35" s="14">
+        <v>20</v>
+      </c>
+      <c r="DA35" s="14">
+        <v>21</v>
+      </c>
+      <c r="DB35" s="14">
+        <v>22</v>
+      </c>
+      <c r="DC35" s="14">
+        <v>23</v>
+      </c>
+      <c r="DD35" s="14">
+        <v>24</v>
+      </c>
+      <c r="DE35" s="14">
+        <v>25</v>
+      </c>
+      <c r="DF35" s="14">
+        <v>26</v>
+      </c>
+      <c r="DG35" s="14">
+        <v>27</v>
+      </c>
+      <c r="DH35" s="14">
+        <v>28</v>
+      </c>
+      <c r="DI35" s="14">
+        <v>29</v>
+      </c>
+      <c r="DJ35" s="14">
+        <v>30</v>
+      </c>
+      <c r="DK35" s="14">
+        <v>31</v>
+      </c>
+      <c r="DL35" s="14">
+        <v>32</v>
+      </c>
+      <c r="DM35" s="14">
+        <v>33</v>
+      </c>
+      <c r="DN35" s="14">
+        <v>34</v>
+      </c>
+      <c r="DO35" s="14">
+        <v>35</v>
+      </c>
+      <c r="DP35" s="14">
+        <v>36</v>
+      </c>
+      <c r="DQ35" s="14">
+        <v>37</v>
+      </c>
+      <c r="DR35" s="14">
+        <v>38</v>
+      </c>
+      <c r="DS35" s="14">
+        <v>39</v>
+      </c>
+      <c r="DT35" s="14">
+        <v>40</v>
+      </c>
+      <c r="DU35" s="14">
+        <v>41</v>
+      </c>
+      <c r="DV35" s="14">
+        <v>42</v>
+      </c>
     </row>
-    <row r="36" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1742,8 +1927,11 @@
       <c r="DV36" s="8">
         <v>3</v>
       </c>
+      <c r="DW36" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="Y37" s="1"/>
@@ -1879,8 +2067,11 @@
       <c r="DV37" s="8">
         <v>3</v>
       </c>
+      <c r="DW37" s="14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2034,8 +2225,11 @@
       <c r="DV38" s="8">
         <v>3</v>
       </c>
+      <c r="DW38" s="14">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="CE39" s="14">
         <v>3</v>
       </c>
@@ -2168,8 +2362,11 @@
       <c r="DV39" s="8">
         <v>3</v>
       </c>
+      <c r="DW39" s="14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="40" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="CE40" s="14">
         <v>4</v>
       </c>
@@ -2302,8 +2499,11 @@
       <c r="DV40" s="8">
         <v>3</v>
       </c>
+      <c r="DW40" s="14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="41" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2507,8 +2707,11 @@
       <c r="DV41" s="8">
         <v>3</v>
       </c>
+      <c r="DW41" s="14">
+        <v>5</v>
+      </c>
     </row>
-    <row r="42" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2701,8 +2904,11 @@
       <c r="DV42" s="8">
         <v>3</v>
       </c>
+      <c r="DW42" s="14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="43" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2894,8 +3100,11 @@
       <c r="DV43" s="8">
         <v>3</v>
       </c>
+      <c r="DW43" s="14">
+        <v>7</v>
+      </c>
     </row>
-    <row r="44" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3087,6 +3296,9 @@
       <c r="DV44" s="8">
         <v>3</v>
       </c>
+      <c r="DW44" s="14">
+        <v>8</v>
+      </c>
       <c r="EA44" s="9">
         <v>0</v>
       </c>
@@ -3098,7 +3310,7 @@
       <c r="EE44" s="21"/>
       <c r="EF44" s="21"/>
     </row>
-    <row r="45" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3291,6 +3503,9 @@
       <c r="DV45" s="8">
         <v>3</v>
       </c>
+      <c r="DW45" s="14">
+        <v>9</v>
+      </c>
       <c r="EA45" s="9">
         <v>1</v>
       </c>
@@ -3302,7 +3517,7 @@
       <c r="EE45" s="21"/>
       <c r="EF45" s="21"/>
     </row>
-    <row r="46" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3501,6 +3716,9 @@
       <c r="DV46" s="8">
         <v>3</v>
       </c>
+      <c r="DW46" s="14">
+        <v>10</v>
+      </c>
       <c r="EA46" s="9">
         <v>2</v>
       </c>
@@ -3512,7 +3730,7 @@
       <c r="EE46" s="21"/>
       <c r="EF46" s="21"/>
     </row>
-    <row r="47" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3684,6 +3902,9 @@
       <c r="DV47" s="8">
         <v>3</v>
       </c>
+      <c r="DW47" s="14">
+        <v>11</v>
+      </c>
       <c r="EA47" s="8">
         <v>3</v>
       </c>
@@ -3694,8 +3915,16 @@
       <c r="ED47" s="21"/>
       <c r="EE47" s="21"/>
       <c r="EF47" s="21"/>
+      <c r="EM47" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="EN47" s="25"/>
+      <c r="EO47" s="25"/>
+      <c r="EP47" s="25"/>
+      <c r="EQ47" s="25"/>
+      <c r="ER47" s="25"/>
     </row>
-    <row r="48" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -3867,6 +4096,9 @@
       <c r="DV48" s="8">
         <v>3</v>
       </c>
+      <c r="DW48" s="14">
+        <v>12</v>
+      </c>
       <c r="EA48" s="9">
         <v>4</v>
       </c>
@@ -3877,8 +4109,18 @@
       <c r="ED48" s="21"/>
       <c r="EE48" s="21"/>
       <c r="EF48" s="21"/>
+      <c r="EM48" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="EN48" s="25"/>
+      <c r="EO48" s="25"/>
+      <c r="EP48" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="EQ48" s="25"/>
+      <c r="ER48" s="25"/>
     </row>
-    <row r="49" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -4070,6 +4312,9 @@
       <c r="DV49" s="8">
         <v>3</v>
       </c>
+      <c r="DW49" s="14">
+        <v>13</v>
+      </c>
       <c r="EA49" s="9">
         <v>5</v>
       </c>
@@ -4080,8 +4325,18 @@
       <c r="ED49" s="21"/>
       <c r="EE49" s="21"/>
       <c r="EF49" s="21"/>
+      <c r="EM49" s="25">
+        <v>5</v>
+      </c>
+      <c r="EN49" s="25"/>
+      <c r="EO49" s="25"/>
+      <c r="EP49" s="25">
+        <v>26</v>
+      </c>
+      <c r="EQ49" s="25"/>
+      <c r="ER49" s="25"/>
     </row>
-    <row r="50" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -4141,8 +4396,8 @@
       <c r="CK50" s="9">
         <v>0</v>
       </c>
-      <c r="CL50" s="8">
-        <v>3</v>
+      <c r="CL50" s="24">
+        <v>13</v>
       </c>
       <c r="CM50" s="8">
         <v>3</v>
@@ -4251,6 +4506,9 @@
       </c>
       <c r="DV50" s="8">
         <v>3</v>
+      </c>
+      <c r="DW50" s="14">
+        <v>14</v>
       </c>
       <c r="EA50" s="15">
         <v>6</v>
@@ -4262,8 +4520,14 @@
       <c r="ED50" s="21"/>
       <c r="EE50" s="21"/>
       <c r="EF50" s="21"/>
+      <c r="EM50" s="25"/>
+      <c r="EN50" s="25"/>
+      <c r="EO50" s="25"/>
+      <c r="EP50" s="25"/>
+      <c r="EQ50" s="25"/>
+      <c r="ER50" s="25"/>
     </row>
-    <row r="51" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4434,6 +4698,9 @@
       <c r="DV51" s="8">
         <v>3</v>
       </c>
+      <c r="DW51" s="14">
+        <v>15</v>
+      </c>
       <c r="EA51" s="16">
         <v>7</v>
       </c>
@@ -4444,8 +4711,14 @@
       <c r="ED51" s="21"/>
       <c r="EE51" s="21"/>
       <c r="EF51" s="21"/>
+      <c r="EM51" s="25"/>
+      <c r="EN51" s="25"/>
+      <c r="EO51" s="25"/>
+      <c r="EP51" s="25"/>
+      <c r="EQ51" s="25"/>
+      <c r="ER51" s="25"/>
     </row>
-    <row r="52" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -4505,8 +4778,8 @@
       <c r="CK52" s="9">
         <v>0</v>
       </c>
-      <c r="CL52" s="8">
-        <v>3</v>
+      <c r="CL52" s="20">
+        <v>11</v>
       </c>
       <c r="CM52" s="8">
         <v>3</v>
@@ -4615,6 +4888,9 @@
       </c>
       <c r="DV52" s="8">
         <v>3</v>
+      </c>
+      <c r="DW52" s="14">
+        <v>16</v>
       </c>
       <c r="EA52" s="17">
         <v>8</v>
@@ -4626,8 +4902,14 @@
       <c r="ED52" s="21"/>
       <c r="EE52" s="21"/>
       <c r="EF52" s="21"/>
+      <c r="EM52" s="25"/>
+      <c r="EN52" s="25"/>
+      <c r="EO52" s="25"/>
+      <c r="EP52" s="25"/>
+      <c r="EQ52" s="25"/>
+      <c r="ER52" s="25"/>
     </row>
-    <row r="53" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -4805,6 +5087,9 @@
       <c r="DV53" s="8">
         <v>3</v>
       </c>
+      <c r="DW53" s="14">
+        <v>17</v>
+      </c>
       <c r="EA53" s="18">
         <v>9</v>
       </c>
@@ -4815,8 +5100,14 @@
       <c r="ED53" s="21"/>
       <c r="EE53" s="21"/>
       <c r="EF53" s="21"/>
+      <c r="EM53" s="25"/>
+      <c r="EN53" s="25"/>
+      <c r="EO53" s="25"/>
+      <c r="EP53" s="25"/>
+      <c r="EQ53" s="25"/>
+      <c r="ER53" s="25"/>
     </row>
-    <row r="54" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -4995,6 +5286,9 @@
       <c r="DV54" s="8">
         <v>3</v>
       </c>
+      <c r="DW54" s="14">
+        <v>18</v>
+      </c>
       <c r="EA54" s="19">
         <v>10</v>
       </c>
@@ -5005,8 +5299,14 @@
       <c r="ED54" s="21"/>
       <c r="EE54" s="21"/>
       <c r="EF54" s="21"/>
+      <c r="EM54" s="25"/>
+      <c r="EN54" s="25"/>
+      <c r="EO54" s="25"/>
+      <c r="EP54" s="25"/>
+      <c r="EQ54" s="25"/>
+      <c r="ER54" s="25"/>
     </row>
-    <row r="55" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5182,6 +5482,9 @@
       <c r="DV55" s="8">
         <v>3</v>
       </c>
+      <c r="DW55" s="14">
+        <v>19</v>
+      </c>
       <c r="EA55" s="20">
         <v>11</v>
       </c>
@@ -5192,8 +5495,14 @@
       <c r="ED55" s="21"/>
       <c r="EE55" s="21"/>
       <c r="EF55" s="21"/>
+      <c r="EM55" s="25"/>
+      <c r="EN55" s="25"/>
+      <c r="EO55" s="25"/>
+      <c r="EP55" s="25"/>
+      <c r="EQ55" s="25"/>
+      <c r="ER55" s="25"/>
     </row>
-    <row r="56" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5251,8 +5560,8 @@
       <c r="CG56" s="8">
         <v>3</v>
       </c>
-      <c r="CH56" s="20">
-        <v>11</v>
+      <c r="CH56" s="24">
+        <v>13</v>
       </c>
       <c r="CI56" s="9">
         <v>0</v>
@@ -5374,8 +5683,27 @@
       <c r="DV56" s="8">
         <v>3</v>
       </c>
+      <c r="DW56" s="14">
+        <v>20</v>
+      </c>
+      <c r="EA56" s="22">
+        <v>12</v>
+      </c>
+      <c r="EB56" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="EC56" s="21"/>
+      <c r="ED56" s="21"/>
+      <c r="EE56" s="21"/>
+      <c r="EF56" s="21"/>
+      <c r="EM56" s="25"/>
+      <c r="EN56" s="25"/>
+      <c r="EO56" s="25"/>
+      <c r="EP56" s="25"/>
+      <c r="EQ56" s="25"/>
+      <c r="ER56" s="25"/>
     </row>
-    <row r="57" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -5438,14 +5766,14 @@
       <c r="CL57" s="8">
         <v>3</v>
       </c>
-      <c r="CM57" s="9">
-        <v>0</v>
-      </c>
-      <c r="CN57" s="9">
-        <v>0</v>
-      </c>
-      <c r="CO57" s="9">
-        <v>0</v>
+      <c r="CM57" s="22">
+        <v>12</v>
+      </c>
+      <c r="CN57" s="22">
+        <v>12</v>
+      </c>
+      <c r="CO57" s="22">
+        <v>12</v>
       </c>
       <c r="CP57" s="8">
         <v>3</v>
@@ -5546,16 +5874,30 @@
       <c r="DV57" s="8">
         <v>3</v>
       </c>
-      <c r="EA57" s="19"/>
+      <c r="DW57" s="14">
+        <v>21</v>
+      </c>
+      <c r="EA57" s="24">
+        <v>13</v>
+      </c>
       <c r="EB57" s="21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="EC57" s="21"/>
       <c r="ED57" s="21"/>
       <c r="EE57" s="21"/>
       <c r="EF57" s="21"/>
+      <c r="EG57" s="21"/>
+      <c r="EH57" s="21"/>
+      <c r="EI57" s="21"/>
+      <c r="EM57" s="25"/>
+      <c r="EN57" s="25"/>
+      <c r="EO57" s="25"/>
+      <c r="EP57" s="25"/>
+      <c r="EQ57" s="25"/>
+      <c r="ER57" s="25"/>
     </row>
-    <row r="58" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -5602,8 +5944,8 @@
       <c r="CN58" s="9">
         <v>0</v>
       </c>
-      <c r="CO58" s="9">
-        <v>0</v>
+      <c r="CO58" s="23">
+        <v>12</v>
       </c>
       <c r="CP58" s="8">
         <v>3</v>
@@ -5704,8 +6046,17 @@
       <c r="DV58" s="8">
         <v>3</v>
       </c>
+      <c r="DW58" s="14">
+        <v>22</v>
+      </c>
+      <c r="EM58" s="26"/>
+      <c r="EN58" s="26"/>
+      <c r="EO58" s="26"/>
+      <c r="EP58" s="26"/>
+      <c r="EQ58" s="26"/>
+      <c r="ER58" s="26"/>
     </row>
-    <row r="59" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -5745,14 +6096,14 @@
       <c r="CL59" s="8">
         <v>3</v>
       </c>
-      <c r="CM59" s="9">
-        <v>0</v>
-      </c>
-      <c r="CN59" s="9">
-        <v>0</v>
-      </c>
-      <c r="CO59" s="9">
-        <v>0</v>
+      <c r="CM59" s="22">
+        <v>12</v>
+      </c>
+      <c r="CN59" s="22">
+        <v>12</v>
+      </c>
+      <c r="CO59" s="22">
+        <v>12</v>
       </c>
       <c r="CP59" s="8">
         <v>3</v>
@@ -5853,8 +6204,27 @@
       <c r="DV59" s="8">
         <v>3</v>
       </c>
+      <c r="DW59" s="14">
+        <v>23</v>
+      </c>
+      <c r="EA59" s="19">
+        <v>14</v>
+      </c>
+      <c r="EB59" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="EC59" s="21"/>
+      <c r="ED59" s="21"/>
+      <c r="EE59" s="21"/>
+      <c r="EF59" s="21"/>
+      <c r="EM59" s="26"/>
+      <c r="EN59" s="26"/>
+      <c r="EO59" s="26"/>
+      <c r="EP59" s="26"/>
+      <c r="EQ59" s="26"/>
+      <c r="ER59" s="26"/>
     </row>
-    <row r="60" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -5900,14 +6270,14 @@
       <c r="CL60" s="8">
         <v>3</v>
       </c>
-      <c r="CM60" s="8">
-        <v>3</v>
+      <c r="CM60" s="20">
+        <v>11</v>
       </c>
       <c r="CN60" s="8">
         <v>3</v>
       </c>
-      <c r="CO60" s="8">
-        <v>3</v>
+      <c r="CO60" s="24">
+        <v>13</v>
       </c>
       <c r="CP60" s="8">
         <v>3</v>
@@ -6008,8 +6378,11 @@
       <c r="DV60" s="8">
         <v>3</v>
       </c>
+      <c r="DW60" s="14">
+        <v>24</v>
+      </c>
     </row>
-    <row r="61" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -6184,8 +6557,11 @@
       <c r="DV61" s="8">
         <v>3</v>
       </c>
+      <c r="DW61" s="14">
+        <v>25</v>
+      </c>
     </row>
-    <row r="62" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -6236,8 +6612,8 @@
       <c r="CJ62" s="9">
         <v>0</v>
       </c>
-      <c r="CK62" s="8">
-        <v>3</v>
+      <c r="CK62" s="19">
+        <v>14</v>
       </c>
       <c r="CL62" s="9">
         <v>0</v>
@@ -6350,8 +6726,11 @@
       <c r="DV62" s="8">
         <v>3</v>
       </c>
+      <c r="DW62" s="14">
+        <v>26</v>
+      </c>
     </row>
-    <row r="63" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -6505,8 +6884,11 @@
       <c r="DV63" s="8">
         <v>3</v>
       </c>
+      <c r="DW63" s="14">
+        <v>27</v>
+      </c>
     </row>
-    <row r="64" spans="2:136" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -6657,6 +7039,9 @@
       </c>
       <c r="DV64" s="8">
         <v>3</v>
+      </c>
+      <c r="DW64" s="14">
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15322,7 +15707,28 @@
       <c r="AH126" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="43">
+    <mergeCell ref="EP57:ER57"/>
+    <mergeCell ref="EP52:ER52"/>
+    <mergeCell ref="EP53:ER53"/>
+    <mergeCell ref="EP54:ER54"/>
+    <mergeCell ref="EP55:ER55"/>
+    <mergeCell ref="EP56:ER56"/>
+    <mergeCell ref="EM47:ER47"/>
+    <mergeCell ref="EM48:EO48"/>
+    <mergeCell ref="EP48:ER48"/>
+    <mergeCell ref="EM49:EO49"/>
+    <mergeCell ref="EM50:EO50"/>
+    <mergeCell ref="EM51:EO51"/>
+    <mergeCell ref="EM52:EO52"/>
+    <mergeCell ref="EM53:EO53"/>
+    <mergeCell ref="EM54:EO54"/>
+    <mergeCell ref="EM55:EO55"/>
+    <mergeCell ref="EM56:EO56"/>
+    <mergeCell ref="EM57:EO57"/>
+    <mergeCell ref="EP49:ER49"/>
+    <mergeCell ref="EP50:ER50"/>
+    <mergeCell ref="EP51:ER51"/>
     <mergeCell ref="EB52:EF52"/>
     <mergeCell ref="EB53:EF53"/>
     <mergeCell ref="EB54:EF54"/>
@@ -15333,8 +15739,10 @@
     <mergeCell ref="AD123:AH123"/>
     <mergeCell ref="AD124:AH124"/>
     <mergeCell ref="AD125:AH125"/>
-    <mergeCell ref="EB57:EF57"/>
+    <mergeCell ref="EB59:EF59"/>
     <mergeCell ref="EB55:EF55"/>
+    <mergeCell ref="EB56:EF56"/>
+    <mergeCell ref="EB57:EI57"/>
     <mergeCell ref="EB49:EF49"/>
     <mergeCell ref="EB50:EF50"/>
     <mergeCell ref="EB51:EF51"/>

</xml_diff>

<commit_message>
Add new letter texture for metal wall
</commit_message>
<xml_diff>
--- a/documents/Map/Map.xlsx
+++ b/documents/Map/Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athicha/Desktop/JavaGameProject/documents/Map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tk-hdd-backup\Data\@KMUTNB WORKs\JavaGameProject\documents\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E4271-A94D-2C44-B0FF-1DD6481D7A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808FA047-2CE0-4762-8DDE-FAA09E057361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19380" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>EMPTY</t>
   </si>
@@ -94,12 +94,15 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>LETTER_METAL_WALL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,15 +152,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +238,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -270,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -316,23 +306,20 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,16 +703,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84092400-AD61-BC4A-9F6E-C24F40418E60}">
   <dimension ref="B2:ER126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH32" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CF36" sqref="CF36:DU64"/>
+    <sheetView tabSelected="1" topLeftCell="J30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CF36" sqref="CF36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="83" max="83" width="2.6640625" customWidth="1"/>
+    <col min="83" max="83" width="2.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -741,16 +728,16 @@
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
     </row>
-    <row r="3" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AM3" s="1"/>
     </row>
-    <row r="4" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z4" s="1"/>
       <c r="AM4" s="1"/>
     </row>
-    <row r="5" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z5" s="1"/>
       <c r="AM5" s="1"/>
       <c r="CW5" s="1"/>
@@ -762,7 +749,7 @@
       <c r="DC5" s="1"/>
       <c r="DD5" s="1"/>
     </row>
-    <row r="6" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AM6" s="1"/>
@@ -770,7 +757,7 @@
       <c r="CZ6" s="1"/>
       <c r="DD6" s="1"/>
     </row>
-    <row r="7" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -811,7 +798,7 @@
       <c r="CW7" s="1"/>
       <c r="DD7" s="1"/>
     </row>
-    <row r="8" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AD8" s="1"/>
@@ -820,7 +807,7 @@
       <c r="CW8" s="1"/>
       <c r="DD8" s="1"/>
     </row>
-    <row r="9" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AD9" s="1"/>
@@ -836,7 +823,7 @@
       <c r="DG9" s="1"/>
       <c r="DH9" s="1"/>
     </row>
-    <row r="10" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R10" s="1"/>
       <c r="V10" s="1"/>
       <c r="Z10" s="1"/>
@@ -875,7 +862,7 @@
       <c r="CZ10" s="1"/>
       <c r="DH10" s="1"/>
     </row>
-    <row r="11" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AM11" s="1"/>
@@ -899,7 +886,7 @@
       <c r="DM11" s="1"/>
       <c r="DN11" s="1"/>
     </row>
-    <row r="12" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AM12" s="1"/>
@@ -918,7 +905,7 @@
       <c r="DL12" s="13"/>
       <c r="DN12" s="1"/>
     </row>
-    <row r="13" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R13" s="1"/>
       <c r="V13" s="1"/>
       <c r="Z13" s="1"/>
@@ -935,7 +922,7 @@
       <c r="DE13" s="1"/>
       <c r="DN13" s="1"/>
     </row>
-    <row r="14" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AM14" s="1"/>
@@ -965,7 +952,7 @@
       <c r="DK14" s="13"/>
       <c r="DN14" s="1"/>
     </row>
-    <row r="15" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5"/>
@@ -1000,7 +987,7 @@
       <c r="DE15" s="1"/>
       <c r="DN15" s="1"/>
     </row>
-    <row r="16" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="J16" s="1"/>
       <c r="R16" s="1"/>
@@ -1020,7 +1007,7 @@
       <c r="DL16" s="1"/>
       <c r="DN16" s="1"/>
     </row>
-    <row r="17" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1079,7 +1066,7 @@
       <c r="DU17" s="1"/>
       <c r="DV17" s="1"/>
     </row>
-    <row r="18" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
       <c r="U18" s="1"/>
       <c r="Z18" s="1"/>
@@ -1123,7 +1110,7 @@
       <c r="DP18" s="1"/>
       <c r="DV18" s="1"/>
     </row>
-    <row r="19" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
       <c r="U19" s="1"/>
       <c r="AJ19" s="1"/>
@@ -1155,7 +1142,7 @@
       <c r="DU19" s="1"/>
       <c r="DV19" s="1"/>
     </row>
-    <row r="20" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="U20" s="1"/>
       <c r="AJ20" s="1"/>
@@ -1179,7 +1166,7 @@
       <c r="DP20" s="1"/>
       <c r="DT20" s="1"/>
     </row>
-    <row r="21" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1207,7 +1194,7 @@
       <c r="DP21" s="1"/>
       <c r="DT21" s="1"/>
     </row>
-    <row r="22" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1259,7 +1246,7 @@
       <c r="DS22" s="1"/>
       <c r="DT22" s="1"/>
     </row>
-    <row r="23" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1293,7 +1280,7 @@
       <c r="DP23" s="1"/>
       <c r="DT23" s="1"/>
     </row>
-    <row r="24" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
       <c r="J24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1321,7 +1308,7 @@
       <c r="DL24" s="1"/>
       <c r="DT24" s="1"/>
     </row>
-    <row r="25" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
       <c r="J25" s="1"/>
       <c r="Q25" s="1"/>
@@ -1347,7 +1334,7 @@
       <c r="DP25" s="1"/>
       <c r="DT25" s="1"/>
     </row>
-    <row r="26" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="Z26" s="5"/>
@@ -1382,7 +1369,7 @@
       <c r="DS26" s="1"/>
       <c r="DT26" s="1"/>
     </row>
-    <row r="27" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="U27" s="1"/>
@@ -1417,7 +1404,7 @@
       <c r="DL27" s="1"/>
       <c r="DS27" s="1"/>
     </row>
-    <row r="28" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
       <c r="J28" s="1"/>
       <c r="Q28" s="1"/>
@@ -1438,7 +1425,7 @@
       <c r="DL28" s="1"/>
       <c r="DS28" s="1"/>
     </row>
-    <row r="29" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
       <c r="J29" s="1"/>
       <c r="Q29" s="1"/>
@@ -1491,7 +1478,7 @@
       <c r="DR29" s="1"/>
       <c r="DS29" s="1"/>
     </row>
-    <row r="30" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="I30" s="1"/>
@@ -1529,7 +1516,7 @@
       <c r="DE30" s="1"/>
       <c r="DQ30" s="1"/>
     </row>
-    <row r="31" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="Y31" s="1"/>
@@ -1557,7 +1544,7 @@
       <c r="DP31" s="1"/>
       <c r="DQ31" s="1"/>
     </row>
-    <row r="32" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1591,7 +1578,7 @@
       <c r="CH32" s="1"/>
       <c r="CQ32" s="1"/>
     </row>
-    <row r="33" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="Y33" s="1"/>
@@ -1609,7 +1596,7 @@
       <c r="CP33" s="1"/>
       <c r="CQ33" s="1"/>
     </row>
-    <row r="34" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
       <c r="I34" s="3"/>
@@ -1625,7 +1612,7 @@
       <c r="AP34" s="1"/>
       <c r="BK34" s="1"/>
     </row>
-    <row r="35" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="Y35" s="1"/>
@@ -1762,7 +1749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1931,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="Y37" s="1"/>
@@ -2071,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2229,7 +2216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CE39" s="14">
         <v>3</v>
       </c>
@@ -2366,7 +2353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CE40" s="14">
         <v>4</v>
       </c>
@@ -2503,7 +2490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2711,7 +2698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2908,7 +2895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -3104,7 +3091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3302,15 +3289,15 @@
       <c r="EA44" s="9">
         <v>0</v>
       </c>
-      <c r="EB44" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="EC44" s="21"/>
-      <c r="ED44" s="21"/>
-      <c r="EE44" s="21"/>
-      <c r="EF44" s="21"/>
+      <c r="EB44" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="EC44" s="25"/>
+      <c r="ED44" s="25"/>
+      <c r="EE44" s="25"/>
+      <c r="EF44" s="25"/>
     </row>
-    <row r="45" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3509,15 +3496,15 @@
       <c r="EA45" s="9">
         <v>1</v>
       </c>
-      <c r="EB45" s="21" t="s">
+      <c r="EB45" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="EC45" s="21"/>
-      <c r="ED45" s="21"/>
-      <c r="EE45" s="21"/>
-      <c r="EF45" s="21"/>
+      <c r="EC45" s="25"/>
+      <c r="ED45" s="25"/>
+      <c r="EE45" s="25"/>
+      <c r="EF45" s="25"/>
     </row>
-    <row r="46" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3722,15 +3709,15 @@
       <c r="EA46" s="9">
         <v>2</v>
       </c>
-      <c r="EB46" s="21" t="s">
+      <c r="EB46" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="EC46" s="21"/>
-      <c r="ED46" s="21"/>
-      <c r="EE46" s="21"/>
-      <c r="EF46" s="21"/>
+      <c r="EC46" s="25"/>
+      <c r="ED46" s="25"/>
+      <c r="EE46" s="25"/>
+      <c r="EF46" s="25"/>
     </row>
-    <row r="47" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3908,23 +3895,23 @@
       <c r="EA47" s="8">
         <v>3</v>
       </c>
-      <c r="EB47" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="EC47" s="21"/>
-      <c r="ED47" s="21"/>
-      <c r="EE47" s="21"/>
-      <c r="EF47" s="21"/>
-      <c r="EM47" s="25" t="s">
+      <c r="EB47" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="EC47" s="25"/>
+      <c r="ED47" s="25"/>
+      <c r="EE47" s="25"/>
+      <c r="EF47" s="25"/>
+      <c r="EM47" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="EN47" s="25"/>
-      <c r="EO47" s="25"/>
-      <c r="EP47" s="25"/>
-      <c r="EQ47" s="25"/>
-      <c r="ER47" s="25"/>
+      <c r="EN47" s="24"/>
+      <c r="EO47" s="24"/>
+      <c r="EP47" s="24"/>
+      <c r="EQ47" s="24"/>
+      <c r="ER47" s="24"/>
     </row>
-    <row r="48" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -4102,25 +4089,25 @@
       <c r="EA48" s="9">
         <v>4</v>
       </c>
-      <c r="EB48" s="21" t="s">
+      <c r="EB48" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="EC48" s="21"/>
-      <c r="ED48" s="21"/>
-      <c r="EE48" s="21"/>
-      <c r="EF48" s="21"/>
-      <c r="EM48" s="25" t="s">
+      <c r="EC48" s="25"/>
+      <c r="ED48" s="25"/>
+      <c r="EE48" s="25"/>
+      <c r="EF48" s="25"/>
+      <c r="EM48" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="EN48" s="25"/>
-      <c r="EO48" s="25"/>
-      <c r="EP48" s="25" t="s">
+      <c r="EN48" s="24"/>
+      <c r="EO48" s="24"/>
+      <c r="EP48" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="EQ48" s="25"/>
-      <c r="ER48" s="25"/>
+      <c r="EQ48" s="24"/>
+      <c r="ER48" s="24"/>
     </row>
-    <row r="49" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -4318,25 +4305,25 @@
       <c r="EA49" s="9">
         <v>5</v>
       </c>
-      <c r="EB49" s="21" t="s">
+      <c r="EB49" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="EC49" s="21"/>
-      <c r="ED49" s="21"/>
-      <c r="EE49" s="21"/>
-      <c r="EF49" s="21"/>
-      <c r="EM49" s="25">
+      <c r="EC49" s="25"/>
+      <c r="ED49" s="25"/>
+      <c r="EE49" s="25"/>
+      <c r="EF49" s="25"/>
+      <c r="EM49" s="24">
         <v>5</v>
       </c>
-      <c r="EN49" s="25"/>
-      <c r="EO49" s="25"/>
-      <c r="EP49" s="25">
+      <c r="EN49" s="24"/>
+      <c r="EO49" s="24"/>
+      <c r="EP49" s="24">
         <v>26</v>
       </c>
-      <c r="EQ49" s="25"/>
-      <c r="ER49" s="25"/>
+      <c r="EQ49" s="24"/>
+      <c r="ER49" s="24"/>
     </row>
-    <row r="50" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -4396,7 +4383,7 @@
       <c r="CK50" s="9">
         <v>0</v>
       </c>
-      <c r="CL50" s="24">
+      <c r="CL50" s="22">
         <v>13</v>
       </c>
       <c r="CM50" s="8">
@@ -4513,21 +4500,21 @@
       <c r="EA50" s="15">
         <v>6</v>
       </c>
-      <c r="EB50" s="21" t="s">
+      <c r="EB50" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="EC50" s="21"/>
-      <c r="ED50" s="21"/>
-      <c r="EE50" s="21"/>
-      <c r="EF50" s="21"/>
-      <c r="EM50" s="25"/>
-      <c r="EN50" s="25"/>
-      <c r="EO50" s="25"/>
-      <c r="EP50" s="25"/>
-      <c r="EQ50" s="25"/>
-      <c r="ER50" s="25"/>
+      <c r="EC50" s="25"/>
+      <c r="ED50" s="25"/>
+      <c r="EE50" s="25"/>
+      <c r="EF50" s="25"/>
+      <c r="EM50" s="24"/>
+      <c r="EN50" s="24"/>
+      <c r="EO50" s="24"/>
+      <c r="EP50" s="24"/>
+      <c r="EQ50" s="24"/>
+      <c r="ER50" s="24"/>
     </row>
-    <row r="51" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4704,21 +4691,21 @@
       <c r="EA51" s="16">
         <v>7</v>
       </c>
-      <c r="EB51" s="21" t="s">
+      <c r="EB51" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="EC51" s="21"/>
-      <c r="ED51" s="21"/>
-      <c r="EE51" s="21"/>
-      <c r="EF51" s="21"/>
-      <c r="EM51" s="25"/>
-      <c r="EN51" s="25"/>
-      <c r="EO51" s="25"/>
-      <c r="EP51" s="25"/>
-      <c r="EQ51" s="25"/>
-      <c r="ER51" s="25"/>
+      <c r="EC51" s="25"/>
+      <c r="ED51" s="25"/>
+      <c r="EE51" s="25"/>
+      <c r="EF51" s="25"/>
+      <c r="EM51" s="24"/>
+      <c r="EN51" s="24"/>
+      <c r="EO51" s="24"/>
+      <c r="EP51" s="24"/>
+      <c r="EQ51" s="24"/>
+      <c r="ER51" s="24"/>
     </row>
-    <row r="52" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -4895,21 +4882,21 @@
       <c r="EA52" s="17">
         <v>8</v>
       </c>
-      <c r="EB52" s="21" t="s">
+      <c r="EB52" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="EC52" s="21"/>
-      <c r="ED52" s="21"/>
-      <c r="EE52" s="21"/>
-      <c r="EF52" s="21"/>
-      <c r="EM52" s="25"/>
-      <c r="EN52" s="25"/>
-      <c r="EO52" s="25"/>
-      <c r="EP52" s="25"/>
-      <c r="EQ52" s="25"/>
-      <c r="ER52" s="25"/>
+      <c r="EC52" s="25"/>
+      <c r="ED52" s="25"/>
+      <c r="EE52" s="25"/>
+      <c r="EF52" s="25"/>
+      <c r="EM52" s="24"/>
+      <c r="EN52" s="24"/>
+      <c r="EO52" s="24"/>
+      <c r="EP52" s="24"/>
+      <c r="EQ52" s="24"/>
+      <c r="ER52" s="24"/>
     </row>
-    <row r="53" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5093,21 +5080,21 @@
       <c r="EA53" s="18">
         <v>9</v>
       </c>
-      <c r="EB53" s="21" t="s">
+      <c r="EB53" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="EC53" s="21"/>
-      <c r="ED53" s="21"/>
-      <c r="EE53" s="21"/>
-      <c r="EF53" s="21"/>
-      <c r="EM53" s="25"/>
-      <c r="EN53" s="25"/>
-      <c r="EO53" s="25"/>
-      <c r="EP53" s="25"/>
-      <c r="EQ53" s="25"/>
-      <c r="ER53" s="25"/>
+      <c r="EC53" s="25"/>
+      <c r="ED53" s="25"/>
+      <c r="EE53" s="25"/>
+      <c r="EF53" s="25"/>
+      <c r="EM53" s="24"/>
+      <c r="EN53" s="24"/>
+      <c r="EO53" s="24"/>
+      <c r="EP53" s="24"/>
+      <c r="EQ53" s="24"/>
+      <c r="ER53" s="24"/>
     </row>
-    <row r="54" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -5292,21 +5279,21 @@
       <c r="EA54" s="19">
         <v>10</v>
       </c>
-      <c r="EB54" s="21" t="s">
+      <c r="EB54" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="EC54" s="21"/>
-      <c r="ED54" s="21"/>
-      <c r="EE54" s="21"/>
-      <c r="EF54" s="21"/>
-      <c r="EM54" s="25"/>
-      <c r="EN54" s="25"/>
-      <c r="EO54" s="25"/>
-      <c r="EP54" s="25"/>
-      <c r="EQ54" s="25"/>
-      <c r="ER54" s="25"/>
+      <c r="EC54" s="25"/>
+      <c r="ED54" s="25"/>
+      <c r="EE54" s="25"/>
+      <c r="EF54" s="25"/>
+      <c r="EM54" s="24"/>
+      <c r="EN54" s="24"/>
+      <c r="EO54" s="24"/>
+      <c r="EP54" s="24"/>
+      <c r="EQ54" s="24"/>
+      <c r="ER54" s="24"/>
     </row>
-    <row r="55" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5488,21 +5475,21 @@
       <c r="EA55" s="20">
         <v>11</v>
       </c>
-      <c r="EB55" s="21" t="s">
+      <c r="EB55" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="EC55" s="21"/>
-      <c r="ED55" s="21"/>
-      <c r="EE55" s="21"/>
-      <c r="EF55" s="21"/>
-      <c r="EM55" s="25"/>
-      <c r="EN55" s="25"/>
-      <c r="EO55" s="25"/>
-      <c r="EP55" s="25"/>
-      <c r="EQ55" s="25"/>
-      <c r="ER55" s="25"/>
+      <c r="EC55" s="25"/>
+      <c r="ED55" s="25"/>
+      <c r="EE55" s="25"/>
+      <c r="EF55" s="25"/>
+      <c r="EM55" s="24"/>
+      <c r="EN55" s="24"/>
+      <c r="EO55" s="24"/>
+      <c r="EP55" s="24"/>
+      <c r="EQ55" s="24"/>
+      <c r="ER55" s="24"/>
     </row>
-    <row r="56" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5560,7 +5547,7 @@
       <c r="CG56" s="8">
         <v>3</v>
       </c>
-      <c r="CH56" s="24">
+      <c r="CH56" s="22">
         <v>13</v>
       </c>
       <c r="CI56" s="9">
@@ -5686,24 +5673,24 @@
       <c r="DW56" s="14">
         <v>20</v>
       </c>
-      <c r="EA56" s="22">
+      <c r="EA56" s="21">
         <v>12</v>
       </c>
-      <c r="EB56" s="21" t="s">
+      <c r="EB56" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="EC56" s="21"/>
-      <c r="ED56" s="21"/>
-      <c r="EE56" s="21"/>
-      <c r="EF56" s="21"/>
-      <c r="EM56" s="25"/>
-      <c r="EN56" s="25"/>
-      <c r="EO56" s="25"/>
-      <c r="EP56" s="25"/>
-      <c r="EQ56" s="25"/>
-      <c r="ER56" s="25"/>
+      <c r="EC56" s="25"/>
+      <c r="ED56" s="25"/>
+      <c r="EE56" s="25"/>
+      <c r="EF56" s="25"/>
+      <c r="EM56" s="24"/>
+      <c r="EN56" s="24"/>
+      <c r="EO56" s="24"/>
+      <c r="EP56" s="24"/>
+      <c r="EQ56" s="24"/>
+      <c r="ER56" s="24"/>
     </row>
-    <row r="57" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -5766,13 +5753,13 @@
       <c r="CL57" s="8">
         <v>3</v>
       </c>
-      <c r="CM57" s="22">
+      <c r="CM57" s="21">
         <v>12</v>
       </c>
-      <c r="CN57" s="22">
+      <c r="CN57" s="21">
         <v>12</v>
       </c>
-      <c r="CO57" s="22">
+      <c r="CO57" s="21">
         <v>12</v>
       </c>
       <c r="CP57" s="8">
@@ -5877,27 +5864,27 @@
       <c r="DW57" s="14">
         <v>21</v>
       </c>
-      <c r="EA57" s="24">
+      <c r="EA57" s="22">
         <v>13</v>
       </c>
-      <c r="EB57" s="21" t="s">
+      <c r="EB57" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="EC57" s="21"/>
-      <c r="ED57" s="21"/>
-      <c r="EE57" s="21"/>
-      <c r="EF57" s="21"/>
-      <c r="EG57" s="21"/>
-      <c r="EH57" s="21"/>
-      <c r="EI57" s="21"/>
-      <c r="EM57" s="25"/>
-      <c r="EN57" s="25"/>
-      <c r="EO57" s="25"/>
-      <c r="EP57" s="25"/>
-      <c r="EQ57" s="25"/>
-      <c r="ER57" s="25"/>
+      <c r="EC57" s="25"/>
+      <c r="ED57" s="25"/>
+      <c r="EE57" s="25"/>
+      <c r="EF57" s="25"/>
+      <c r="EG57" s="25"/>
+      <c r="EH57" s="25"/>
+      <c r="EI57" s="25"/>
+      <c r="EM57" s="24"/>
+      <c r="EN57" s="24"/>
+      <c r="EO57" s="24"/>
+      <c r="EP57" s="24"/>
+      <c r="EQ57" s="24"/>
+      <c r="ER57" s="24"/>
     </row>
-    <row r="58" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -5944,8 +5931,8 @@
       <c r="CN58" s="9">
         <v>0</v>
       </c>
-      <c r="CO58" s="23">
-        <v>12</v>
+      <c r="CO58" s="19">
+        <v>15</v>
       </c>
       <c r="CP58" s="8">
         <v>3</v>
@@ -6049,14 +6036,14 @@
       <c r="DW58" s="14">
         <v>22</v>
       </c>
-      <c r="EM58" s="26"/>
-      <c r="EN58" s="26"/>
-      <c r="EO58" s="26"/>
-      <c r="EP58" s="26"/>
-      <c r="EQ58" s="26"/>
-      <c r="ER58" s="26"/>
+      <c r="EM58" s="23"/>
+      <c r="EN58" s="23"/>
+      <c r="EO58" s="23"/>
+      <c r="EP58" s="23"/>
+      <c r="EQ58" s="23"/>
+      <c r="ER58" s="23"/>
     </row>
-    <row r="59" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -6096,13 +6083,13 @@
       <c r="CL59" s="8">
         <v>3</v>
       </c>
-      <c r="CM59" s="22">
+      <c r="CM59" s="21">
         <v>12</v>
       </c>
-      <c r="CN59" s="22">
+      <c r="CN59" s="21">
         <v>12</v>
       </c>
-      <c r="CO59" s="22">
+      <c r="CO59" s="21">
         <v>12</v>
       </c>
       <c r="CP59" s="8">
@@ -6210,21 +6197,21 @@
       <c r="EA59" s="19">
         <v>14</v>
       </c>
-      <c r="EB59" s="21" t="s">
+      <c r="EB59" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="EC59" s="21"/>
-      <c r="ED59" s="21"/>
-      <c r="EE59" s="21"/>
-      <c r="EF59" s="21"/>
-      <c r="EM59" s="26"/>
-      <c r="EN59" s="26"/>
-      <c r="EO59" s="26"/>
-      <c r="EP59" s="26"/>
-      <c r="EQ59" s="26"/>
-      <c r="ER59" s="26"/>
+      <c r="EC59" s="25"/>
+      <c r="ED59" s="25"/>
+      <c r="EE59" s="25"/>
+      <c r="EF59" s="25"/>
+      <c r="EM59" s="23"/>
+      <c r="EN59" s="23"/>
+      <c r="EO59" s="23"/>
+      <c r="EP59" s="23"/>
+      <c r="EQ59" s="23"/>
+      <c r="ER59" s="23"/>
     </row>
-    <row r="60" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -6276,7 +6263,7 @@
       <c r="CN60" s="8">
         <v>3</v>
       </c>
-      <c r="CO60" s="24">
+      <c r="CO60" s="22">
         <v>13</v>
       </c>
       <c r="CP60" s="8">
@@ -6381,8 +6368,22 @@
       <c r="DW60" s="14">
         <v>24</v>
       </c>
+      <c r="EA60" s="19">
+        <v>15</v>
+      </c>
+      <c r="EB60" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="EC60" s="25"/>
+      <c r="ED60" s="25"/>
+      <c r="EE60" s="25"/>
+      <c r="EF60" s="25"/>
+      <c r="EG60" s="25"/>
+      <c r="EH60" s="25"/>
+      <c r="EI60" s="25"/>
+      <c r="EJ60" s="25"/>
     </row>
-    <row r="61" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -6561,7 +6562,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -6730,7 +6731,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -6888,7 +6889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -7044,7 +7045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -7194,7 +7195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -7229,7 +7230,7 @@
       <c r="BS66" s="1"/>
       <c r="BT66" s="1"/>
     </row>
-    <row r="67" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -7251,7 +7252,7 @@
       <c r="BS67" s="1"/>
       <c r="BT67" s="1"/>
     </row>
-    <row r="68" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -7282,7 +7283,7 @@
       <c r="BS68" s="1"/>
       <c r="BT68" s="1"/>
     </row>
-    <row r="69" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -7323,7 +7324,7 @@
       <c r="BS69" s="1"/>
       <c r="BT69" s="1"/>
     </row>
-    <row r="70" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -7349,7 +7350,7 @@
       <c r="BS70" s="1"/>
       <c r="BT70" s="1"/>
     </row>
-    <row r="71" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -7393,7 +7394,7 @@
       <c r="BS71" s="1"/>
       <c r="BT71" s="1"/>
     </row>
-    <row r="72" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="R72" s="1"/>
@@ -7421,7 +7422,7 @@
       <c r="BS72" s="1"/>
       <c r="BT72" s="1"/>
     </row>
-    <row r="73" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="E73" s="2"/>
@@ -7457,7 +7458,7 @@
       <c r="BS73" s="1"/>
       <c r="BT73" s="1"/>
     </row>
-    <row r="74" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="R74" s="1"/>
@@ -7485,7 +7486,7 @@
       <c r="BS74" s="1"/>
       <c r="BT74" s="1"/>
     </row>
-    <row r="75" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -7539,7 +7540,7 @@
       <c r="BS75" s="1"/>
       <c r="BT75" s="1"/>
     </row>
-    <row r="76" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -7594,7 +7595,7 @@
       <c r="BS76" s="1"/>
       <c r="BT76" s="1"/>
     </row>
-    <row r="77" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -7667,7 +7668,7 @@
       <c r="BS77" s="1"/>
       <c r="BT77" s="1"/>
     </row>
-    <row r="79" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="8">
         <v>3</v>
       </c>
@@ -7882,7 +7883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="8">
         <v>3</v>
       </c>
@@ -8097,7 +8098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="8">
         <v>3</v>
       </c>
@@ -8312,7 +8313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="8">
         <v>3</v>
       </c>
@@ -8527,7 +8528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="8">
         <v>3</v>
       </c>
@@ -8742,7 +8743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8">
         <v>3</v>
       </c>
@@ -8957,7 +8958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="8">
         <v>3</v>
       </c>
@@ -9172,7 +9173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8">
         <v>3</v>
       </c>
@@ -9387,7 +9388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="8">
         <v>3</v>
       </c>
@@ -9602,7 +9603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8">
         <v>3</v>
       </c>
@@ -9817,7 +9818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="8">
         <v>3</v>
       </c>
@@ -10032,7 +10033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="8">
         <v>3</v>
       </c>
@@ -10247,7 +10248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="8">
         <v>3</v>
       </c>
@@ -10462,7 +10463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="8">
         <v>3</v>
       </c>
@@ -10677,7 +10678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="8">
         <v>3</v>
       </c>
@@ -10892,7 +10893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="8">
         <v>3</v>
       </c>
@@ -11107,7 +11108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="8">
         <v>3</v>
       </c>
@@ -11322,7 +11323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="8">
         <v>3</v>
       </c>
@@ -11537,7 +11538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="8">
         <v>3</v>
       </c>
@@ -11752,7 +11753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="8">
         <v>3</v>
       </c>
@@ -11967,7 +11968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="8">
         <v>3</v>
       </c>
@@ -12182,7 +12183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="8">
         <v>3</v>
       </c>
@@ -12397,7 +12398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="8">
         <v>3</v>
       </c>
@@ -12612,7 +12613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="8">
         <v>3</v>
       </c>
@@ -12827,7 +12828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="8">
         <v>3</v>
       </c>
@@ -13042,7 +13043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="8">
         <v>3</v>
       </c>
@@ -13257,7 +13258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="8">
         <v>3</v>
       </c>
@@ -13472,7 +13473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="8">
         <v>3</v>
       </c>
@@ -13687,7 +13688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="8">
         <v>3</v>
       </c>
@@ -13902,7 +13903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="8">
         <v>3</v>
       </c>
@@ -14117,7 +14118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="8">
         <v>3</v>
       </c>
@@ -14332,7 +14333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="8">
         <v>3</v>
       </c>
@@ -14547,7 +14548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="8">
         <v>3</v>
       </c>
@@ -14762,7 +14763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="8">
         <v>3</v>
       </c>
@@ -14977,7 +14978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="8">
         <v>3</v>
       </c>
@@ -15192,7 +15193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="8">
         <v>3</v>
       </c>
@@ -15407,7 +15408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="8">
         <v>3</v>
       </c>
@@ -15622,113 +15623,100 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC120">
         <v>0</v>
       </c>
-      <c r="AD120" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE120" s="21"/>
-      <c r="AF120" s="21"/>
-      <c r="AG120" s="21"/>
-      <c r="AH120" s="21"/>
+      <c r="AD120" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE120" s="25"/>
+      <c r="AF120" s="25"/>
+      <c r="AG120" s="25"/>
+      <c r="AH120" s="25"/>
     </row>
-    <row r="121" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC121">
         <v>1</v>
       </c>
-      <c r="AD121" s="21" t="s">
+      <c r="AD121" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AE121" s="21"/>
-      <c r="AF121" s="21"/>
-      <c r="AG121" s="21"/>
-      <c r="AH121" s="21"/>
+      <c r="AE121" s="25"/>
+      <c r="AF121" s="25"/>
+      <c r="AG121" s="25"/>
+      <c r="AH121" s="25"/>
     </row>
-    <row r="122" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC122">
         <v>2</v>
       </c>
-      <c r="AD122" s="21" t="s">
+      <c r="AD122" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AE122" s="21"/>
-      <c r="AF122" s="21"/>
-      <c r="AG122" s="21"/>
-      <c r="AH122" s="21"/>
+      <c r="AE122" s="25"/>
+      <c r="AF122" s="25"/>
+      <c r="AG122" s="25"/>
+      <c r="AH122" s="25"/>
     </row>
-    <row r="123" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC123">
         <v>3</v>
       </c>
-      <c r="AD123" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE123" s="21"/>
-      <c r="AF123" s="21"/>
-      <c r="AG123" s="21"/>
-      <c r="AH123" s="21"/>
+      <c r="AD123" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE123" s="25"/>
+      <c r="AF123" s="25"/>
+      <c r="AG123" s="25"/>
+      <c r="AH123" s="25"/>
     </row>
-    <row r="124" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC124">
         <v>4</v>
       </c>
-      <c r="AD124" s="21" t="s">
+      <c r="AD124" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AE124" s="21"/>
-      <c r="AF124" s="21"/>
-      <c r="AG124" s="21"/>
-      <c r="AH124" s="21"/>
+      <c r="AE124" s="25"/>
+      <c r="AF124" s="25"/>
+      <c r="AG124" s="25"/>
+      <c r="AH124" s="25"/>
     </row>
-    <row r="125" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC125">
         <v>5</v>
       </c>
-      <c r="AD125" s="21" t="s">
+      <c r="AD125" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AE125" s="21"/>
-      <c r="AF125" s="21"/>
-      <c r="AG125" s="21"/>
-      <c r="AH125" s="21"/>
+      <c r="AE125" s="25"/>
+      <c r="AF125" s="25"/>
+      <c r="AG125" s="25"/>
+      <c r="AH125" s="25"/>
     </row>
-    <row r="126" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC126">
         <v>6</v>
       </c>
-      <c r="AD126" s="21" t="s">
+      <c r="AD126" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AE126" s="21"/>
-      <c r="AF126" s="21"/>
-      <c r="AG126" s="21"/>
-      <c r="AH126" s="21"/>
+      <c r="AE126" s="25"/>
+      <c r="AF126" s="25"/>
+      <c r="AG126" s="25"/>
+      <c r="AH126" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="EP57:ER57"/>
-    <mergeCell ref="EP52:ER52"/>
-    <mergeCell ref="EP53:ER53"/>
-    <mergeCell ref="EP54:ER54"/>
-    <mergeCell ref="EP55:ER55"/>
-    <mergeCell ref="EP56:ER56"/>
-    <mergeCell ref="EM47:ER47"/>
-    <mergeCell ref="EM48:EO48"/>
-    <mergeCell ref="EP48:ER48"/>
-    <mergeCell ref="EM49:EO49"/>
-    <mergeCell ref="EM50:EO50"/>
-    <mergeCell ref="EM51:EO51"/>
-    <mergeCell ref="EM52:EO52"/>
-    <mergeCell ref="EM53:EO53"/>
-    <mergeCell ref="EM54:EO54"/>
-    <mergeCell ref="EM55:EO55"/>
-    <mergeCell ref="EM56:EO56"/>
-    <mergeCell ref="EM57:EO57"/>
-    <mergeCell ref="EP49:ER49"/>
-    <mergeCell ref="EP50:ER50"/>
-    <mergeCell ref="EP51:ER51"/>
+  <mergeCells count="44">
+    <mergeCell ref="EB49:EF49"/>
+    <mergeCell ref="EB50:EF50"/>
+    <mergeCell ref="EB51:EF51"/>
+    <mergeCell ref="EB44:EF44"/>
+    <mergeCell ref="EB45:EF45"/>
+    <mergeCell ref="EB46:EF46"/>
+    <mergeCell ref="EB47:EF47"/>
+    <mergeCell ref="EB48:EF48"/>
     <mergeCell ref="EB52:EF52"/>
     <mergeCell ref="EB53:EF53"/>
     <mergeCell ref="EB54:EF54"/>
@@ -15743,14 +15731,28 @@
     <mergeCell ref="EB55:EF55"/>
     <mergeCell ref="EB56:EF56"/>
     <mergeCell ref="EB57:EI57"/>
-    <mergeCell ref="EB49:EF49"/>
-    <mergeCell ref="EB50:EF50"/>
-    <mergeCell ref="EB51:EF51"/>
-    <mergeCell ref="EB44:EF44"/>
-    <mergeCell ref="EB45:EF45"/>
-    <mergeCell ref="EB46:EF46"/>
-    <mergeCell ref="EB47:EF47"/>
-    <mergeCell ref="EB48:EF48"/>
+    <mergeCell ref="EB60:EJ60"/>
+    <mergeCell ref="EM56:EO56"/>
+    <mergeCell ref="EM57:EO57"/>
+    <mergeCell ref="EP49:ER49"/>
+    <mergeCell ref="EP50:ER50"/>
+    <mergeCell ref="EP51:ER51"/>
+    <mergeCell ref="EM51:EO51"/>
+    <mergeCell ref="EM52:EO52"/>
+    <mergeCell ref="EM53:EO53"/>
+    <mergeCell ref="EM54:EO54"/>
+    <mergeCell ref="EM55:EO55"/>
+    <mergeCell ref="EM47:ER47"/>
+    <mergeCell ref="EM48:EO48"/>
+    <mergeCell ref="EP48:ER48"/>
+    <mergeCell ref="EM49:EO49"/>
+    <mergeCell ref="EM50:EO50"/>
+    <mergeCell ref="EP57:ER57"/>
+    <mergeCell ref="EP52:ER52"/>
+    <mergeCell ref="EP53:ER53"/>
+    <mergeCell ref="EP54:ER54"/>
+    <mergeCell ref="EP55:ER55"/>
+    <mergeCell ref="EP56:ER56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add new textures and update Map.csv
</commit_message>
<xml_diff>
--- a/documents/Map/Map.xlsx
+++ b/documents/Map/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tk-hdd-backup\Data\@KMUTNB WORKs\JavaGameProject\documents\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808FA047-2CE0-4762-8DDE-FAA09E057361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3490885-BE56-4A39-976C-7B609AE651CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>EMPTY</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>LETTER_METAL_WALL</t>
+  </si>
+  <si>
+    <t>GET OUT</t>
+  </si>
+  <si>
+    <t>LETTER_BLOOD_WALL</t>
   </si>
 </sst>
 </file>
@@ -316,10 +322,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84092400-AD61-BC4A-9F6E-C24F40418E60}">
   <dimension ref="B2:ER126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CF36" sqref="CF36"/>
+    <sheetView tabSelected="1" topLeftCell="L31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="DR45" sqref="DR45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1839,17 +1845,17 @@
       <c r="CW36" s="8">
         <v>3</v>
       </c>
-      <c r="CX36" s="8">
-        <v>3</v>
-      </c>
-      <c r="CY36" s="8">
-        <v>3</v>
+      <c r="CX36" s="21">
+        <v>12</v>
+      </c>
+      <c r="CY36" s="21">
+        <v>12</v>
       </c>
       <c r="CZ36" s="8">
         <v>3</v>
       </c>
-      <c r="DA36" s="8">
-        <v>3</v>
+      <c r="DA36" s="17">
+        <v>8</v>
       </c>
       <c r="DB36" s="8">
         <v>3</v>
@@ -1997,8 +2003,8 @@
       <c r="DC37" s="9">
         <v>0</v>
       </c>
-      <c r="DD37" s="8">
-        <v>3</v>
+      <c r="DD37" s="21">
+        <v>12</v>
       </c>
       <c r="DE37" s="8">
         <v>3</v>
@@ -2122,20 +2128,20 @@
       <c r="CR38" s="8">
         <v>3</v>
       </c>
-      <c r="CS38" s="8">
-        <v>3</v>
+      <c r="CS38" s="22">
+        <v>13</v>
       </c>
       <c r="CT38" s="8">
         <v>3</v>
       </c>
-      <c r="CU38" s="8">
-        <v>3</v>
+      <c r="CU38" s="20">
+        <v>11</v>
       </c>
       <c r="CV38" s="8">
         <v>3</v>
       </c>
-      <c r="CW38" s="8">
-        <v>3</v>
+      <c r="CW38" s="18">
+        <v>9</v>
       </c>
       <c r="CX38" s="9">
         <v>0</v>
@@ -2155,8 +2161,8 @@
       <c r="DC38" s="9">
         <v>0</v>
       </c>
-      <c r="DD38" s="8">
-        <v>3</v>
+      <c r="DD38" s="21">
+        <v>12</v>
       </c>
       <c r="DE38" s="8">
         <v>3</v>
@@ -2292,8 +2298,8 @@
       <c r="DC39" s="9">
         <v>0</v>
       </c>
-      <c r="DD39" s="8">
-        <v>3</v>
+      <c r="DD39" s="21">
+        <v>12</v>
       </c>
       <c r="DE39" s="8">
         <v>3</v>
@@ -2390,8 +2396,8 @@
       <c r="CP40" s="8">
         <v>3</v>
       </c>
-      <c r="CQ40" s="8">
-        <v>3</v>
+      <c r="CQ40" s="20">
+        <v>11</v>
       </c>
       <c r="CR40" s="9">
         <v>0</v>
@@ -2408,8 +2414,8 @@
       <c r="CV40" s="9">
         <v>0</v>
       </c>
-      <c r="CW40" s="8">
-        <v>3</v>
+      <c r="CW40" s="18">
+        <v>9</v>
       </c>
       <c r="CX40" s="9">
         <v>0</v>
@@ -2435,8 +2441,8 @@
       <c r="DE40" s="8">
         <v>3</v>
       </c>
-      <c r="DF40" s="8">
-        <v>3</v>
+      <c r="DF40" s="22">
+        <v>16</v>
       </c>
       <c r="DG40" s="8">
         <v>3</v>
@@ -2607,8 +2613,8 @@
       <c r="CS41" s="9">
         <v>0</v>
       </c>
-      <c r="CT41" s="8">
-        <v>3</v>
+      <c r="CT41" s="21">
+        <v>12</v>
       </c>
       <c r="CU41" s="9">
         <v>0</v>
@@ -2649,8 +2655,8 @@
       <c r="DG41" s="9">
         <v>0</v>
       </c>
-      <c r="DH41" s="8">
-        <v>3</v>
+      <c r="DH41" s="16">
+        <v>7</v>
       </c>
       <c r="DI41" s="8">
         <v>3</v>
@@ -2795,8 +2801,8 @@
       <c r="CP42" s="8">
         <v>3</v>
       </c>
-      <c r="CQ42" s="8">
-        <v>3</v>
+      <c r="CQ42" s="16">
+        <v>7</v>
       </c>
       <c r="CR42" s="9">
         <v>0</v>
@@ -2813,8 +2819,8 @@
       <c r="CV42" s="9">
         <v>0</v>
       </c>
-      <c r="CW42" s="8">
-        <v>3</v>
+      <c r="CW42" s="18">
+        <v>9</v>
       </c>
       <c r="CX42" s="9">
         <v>0</v>
@@ -2831,8 +2837,8 @@
       <c r="DB42" s="8">
         <v>3</v>
       </c>
-      <c r="DC42" s="8">
-        <v>3</v>
+      <c r="DC42" s="17">
+        <v>8</v>
       </c>
       <c r="DD42" s="8">
         <v>3</v>
@@ -2852,8 +2858,8 @@
       <c r="DI42" s="8">
         <v>3</v>
       </c>
-      <c r="DJ42" s="8">
-        <v>3</v>
+      <c r="DJ42" s="17">
+        <v>8</v>
       </c>
       <c r="DK42" s="8">
         <v>3</v>
@@ -3000,8 +3006,8 @@
       <c r="CS43" s="9">
         <v>0</v>
       </c>
-      <c r="CT43" s="8">
-        <v>3</v>
+      <c r="CT43" s="21">
+        <v>12</v>
       </c>
       <c r="CU43" s="9">
         <v>0</v>
@@ -3033,8 +3039,8 @@
       <c r="DD43" s="8">
         <v>3</v>
       </c>
-      <c r="DE43" s="8">
-        <v>3</v>
+      <c r="DE43" s="21">
+        <v>12</v>
       </c>
       <c r="DF43" s="9">
         <v>0</v>
@@ -3187,8 +3193,8 @@
       <c r="CP44" s="8">
         <v>3</v>
       </c>
-      <c r="CQ44" s="8">
-        <v>3</v>
+      <c r="CQ44" s="20">
+        <v>11</v>
       </c>
       <c r="CR44" s="9">
         <v>0</v>
@@ -3205,8 +3211,8 @@
       <c r="CV44" s="9">
         <v>0</v>
       </c>
-      <c r="CW44" s="8">
-        <v>3</v>
+      <c r="CW44" s="18">
+        <v>9</v>
       </c>
       <c r="CX44" s="9">
         <v>0</v>
@@ -3214,8 +3220,8 @@
       <c r="CY44" s="9">
         <v>0</v>
       </c>
-      <c r="CZ44" s="8">
-        <v>3</v>
+      <c r="CZ44" s="17">
+        <v>8</v>
       </c>
       <c r="DA44" s="8">
         <v>3</v>
@@ -3229,8 +3235,8 @@
       <c r="DD44" s="8">
         <v>3</v>
       </c>
-      <c r="DE44" s="8">
-        <v>3</v>
+      <c r="DE44" s="21">
+        <v>12</v>
       </c>
       <c r="DF44" s="9">
         <v>0</v>
@@ -3289,13 +3295,13 @@
       <c r="EA44" s="9">
         <v>0</v>
       </c>
-      <c r="EB44" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="EC44" s="25"/>
-      <c r="ED44" s="25"/>
-      <c r="EE44" s="25"/>
-      <c r="EF44" s="25"/>
+      <c r="EB44" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="EC44" s="24"/>
+      <c r="ED44" s="24"/>
+      <c r="EE44" s="24"/>
+      <c r="EF44" s="24"/>
     </row>
     <row r="45" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
@@ -3496,13 +3502,13 @@
       <c r="EA45" s="9">
         <v>1</v>
       </c>
-      <c r="EB45" s="25" t="s">
+      <c r="EB45" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="EC45" s="25"/>
-      <c r="ED45" s="25"/>
-      <c r="EE45" s="25"/>
-      <c r="EF45" s="25"/>
+      <c r="EC45" s="24"/>
+      <c r="ED45" s="24"/>
+      <c r="EE45" s="24"/>
+      <c r="EF45" s="24"/>
     </row>
     <row r="46" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
@@ -3613,8 +3619,8 @@
       <c r="CR46" s="8">
         <v>3</v>
       </c>
-      <c r="CS46" s="8">
-        <v>3</v>
+      <c r="CS46" s="17">
+        <v>8</v>
       </c>
       <c r="CT46" s="8">
         <v>3</v>
@@ -3625,8 +3631,8 @@
       <c r="CV46" s="8">
         <v>3</v>
       </c>
-      <c r="CW46" s="8">
-        <v>3</v>
+      <c r="CW46" s="18">
+        <v>9</v>
       </c>
       <c r="CX46" s="9">
         <v>0</v>
@@ -3676,8 +3682,8 @@
       <c r="DM46" s="9">
         <v>0</v>
       </c>
-      <c r="DN46" s="8">
-        <v>3</v>
+      <c r="DN46" s="22">
+        <v>16</v>
       </c>
       <c r="DO46" s="8">
         <v>3</v>
@@ -3709,13 +3715,13 @@
       <c r="EA46" s="9">
         <v>2</v>
       </c>
-      <c r="EB46" s="25" t="s">
+      <c r="EB46" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="EC46" s="25"/>
-      <c r="ED46" s="25"/>
-      <c r="EE46" s="25"/>
-      <c r="EF46" s="25"/>
+      <c r="EC46" s="24"/>
+      <c r="ED46" s="24"/>
+      <c r="EE46" s="24"/>
+      <c r="EF46" s="24"/>
     </row>
     <row r="47" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
@@ -3835,8 +3841,8 @@
       <c r="DD47" s="8">
         <v>3</v>
       </c>
-      <c r="DE47" s="8">
-        <v>3</v>
+      <c r="DE47" s="17">
+        <v>8</v>
       </c>
       <c r="DF47" s="9">
         <v>0</v>
@@ -3895,21 +3901,21 @@
       <c r="EA47" s="8">
         <v>3</v>
       </c>
-      <c r="EB47" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="EC47" s="25"/>
-      <c r="ED47" s="25"/>
-      <c r="EE47" s="25"/>
-      <c r="EF47" s="25"/>
-      <c r="EM47" s="24" t="s">
+      <c r="EB47" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="EC47" s="24"/>
+      <c r="ED47" s="24"/>
+      <c r="EE47" s="24"/>
+      <c r="EF47" s="24"/>
+      <c r="EM47" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="EN47" s="24"/>
-      <c r="EO47" s="24"/>
-      <c r="EP47" s="24"/>
-      <c r="EQ47" s="24"/>
-      <c r="ER47" s="24"/>
+      <c r="EN47" s="25"/>
+      <c r="EO47" s="25"/>
+      <c r="EP47" s="25"/>
+      <c r="EQ47" s="25"/>
+      <c r="ER47" s="25"/>
     </row>
     <row r="48" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
@@ -3993,8 +3999,8 @@
       <c r="CR48" s="8">
         <v>3</v>
       </c>
-      <c r="CS48" s="8">
-        <v>3</v>
+      <c r="CS48" s="20">
+        <v>11</v>
       </c>
       <c r="CT48" s="9">
         <v>0</v>
@@ -4065,20 +4071,20 @@
       <c r="DP48" s="8">
         <v>3</v>
       </c>
-      <c r="DQ48" s="8">
-        <v>3</v>
-      </c>
-      <c r="DR48" s="8">
-        <v>3</v>
-      </c>
-      <c r="DS48" s="8">
-        <v>3</v>
-      </c>
-      <c r="DT48" s="8">
-        <v>3</v>
-      </c>
-      <c r="DU48" s="8">
-        <v>3</v>
+      <c r="DQ48" s="21">
+        <v>12</v>
+      </c>
+      <c r="DR48" s="22">
+        <v>16</v>
+      </c>
+      <c r="DS48" s="21">
+        <v>12</v>
+      </c>
+      <c r="DT48" s="21">
+        <v>12</v>
+      </c>
+      <c r="DU48" s="21">
+        <v>12</v>
       </c>
       <c r="DV48" s="8">
         <v>3</v>
@@ -4089,23 +4095,23 @@
       <c r="EA48" s="9">
         <v>4</v>
       </c>
-      <c r="EB48" s="25" t="s">
+      <c r="EB48" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="EC48" s="25"/>
-      <c r="ED48" s="25"/>
-      <c r="EE48" s="25"/>
-      <c r="EF48" s="25"/>
-      <c r="EM48" s="24" t="s">
+      <c r="EC48" s="24"/>
+      <c r="ED48" s="24"/>
+      <c r="EE48" s="24"/>
+      <c r="EF48" s="24"/>
+      <c r="EM48" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="EN48" s="24"/>
-      <c r="EO48" s="24"/>
-      <c r="EP48" s="24" t="s">
+      <c r="EN48" s="25"/>
+      <c r="EO48" s="25"/>
+      <c r="EP48" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="EQ48" s="24"/>
-      <c r="ER48" s="24"/>
+      <c r="EQ48" s="25"/>
+      <c r="ER48" s="25"/>
     </row>
     <row r="49" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
@@ -4209,8 +4215,8 @@
       <c r="CR49" s="8">
         <v>3</v>
       </c>
-      <c r="CS49" s="8">
-        <v>3</v>
+      <c r="CS49" s="20">
+        <v>11</v>
       </c>
       <c r="CT49" s="9">
         <v>0</v>
@@ -4245,8 +4251,8 @@
       <c r="DD49" s="8">
         <v>3</v>
       </c>
-      <c r="DE49" s="8">
-        <v>3</v>
+      <c r="DE49" s="22">
+        <v>17</v>
       </c>
       <c r="DF49" s="9">
         <v>0</v>
@@ -4278,8 +4284,8 @@
       <c r="DO49" s="8">
         <v>3</v>
       </c>
-      <c r="DP49" s="8">
-        <v>3</v>
+      <c r="DP49" s="21">
+        <v>12</v>
       </c>
       <c r="DQ49" s="9">
         <v>0</v>
@@ -4296,8 +4302,8 @@
       <c r="DU49" s="9">
         <v>0</v>
       </c>
-      <c r="DV49" s="8">
-        <v>3</v>
+      <c r="DV49" s="19">
+        <v>10</v>
       </c>
       <c r="DW49" s="14">
         <v>13</v>
@@ -4305,23 +4311,23 @@
       <c r="EA49" s="9">
         <v>5</v>
       </c>
-      <c r="EB49" s="25" t="s">
+      <c r="EB49" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="EC49" s="25"/>
-      <c r="ED49" s="25"/>
-      <c r="EE49" s="25"/>
-      <c r="EF49" s="25"/>
-      <c r="EM49" s="24">
+      <c r="EC49" s="24"/>
+      <c r="ED49" s="24"/>
+      <c r="EE49" s="24"/>
+      <c r="EF49" s="24"/>
+      <c r="EM49" s="25">
         <v>5</v>
       </c>
-      <c r="EN49" s="24"/>
-      <c r="EO49" s="24"/>
-      <c r="EP49" s="24">
+      <c r="EN49" s="25"/>
+      <c r="EO49" s="25"/>
+      <c r="EP49" s="25">
         <v>26</v>
       </c>
-      <c r="EQ49" s="24"/>
-      <c r="ER49" s="24"/>
+      <c r="EQ49" s="25"/>
+      <c r="ER49" s="25"/>
     </row>
     <row r="50" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
@@ -4425,8 +4431,8 @@
       <c r="CY50" s="9">
         <v>0</v>
       </c>
-      <c r="CZ50" s="8">
-        <v>3</v>
+      <c r="CZ50" s="22">
+        <v>16</v>
       </c>
       <c r="DA50" s="8">
         <v>3</v>
@@ -4464,8 +4470,8 @@
       <c r="DL50" s="8">
         <v>3</v>
       </c>
-      <c r="DM50" s="8">
-        <v>3</v>
+      <c r="DM50" s="17">
+        <v>8</v>
       </c>
       <c r="DN50" s="8">
         <v>3</v>
@@ -4473,8 +4479,8 @@
       <c r="DO50" s="8">
         <v>3</v>
       </c>
-      <c r="DP50" s="8">
-        <v>3</v>
+      <c r="DP50" s="22">
+        <v>13</v>
       </c>
       <c r="DQ50" s="9">
         <v>0</v>
@@ -4485,11 +4491,11 @@
       <c r="DS50" s="9">
         <v>0</v>
       </c>
-      <c r="DT50" s="8">
-        <v>3</v>
-      </c>
-      <c r="DU50" s="8">
-        <v>3</v>
+      <c r="DT50" s="21">
+        <v>12</v>
+      </c>
+      <c r="DU50" s="21">
+        <v>12</v>
       </c>
       <c r="DV50" s="8">
         <v>3</v>
@@ -4500,19 +4506,19 @@
       <c r="EA50" s="15">
         <v>6</v>
       </c>
-      <c r="EB50" s="25" t="s">
+      <c r="EB50" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="EC50" s="25"/>
-      <c r="ED50" s="25"/>
-      <c r="EE50" s="25"/>
-      <c r="EF50" s="25"/>
-      <c r="EM50" s="24"/>
-      <c r="EN50" s="24"/>
-      <c r="EO50" s="24"/>
-      <c r="EP50" s="24"/>
-      <c r="EQ50" s="24"/>
-      <c r="ER50" s="24"/>
+      <c r="EC50" s="24"/>
+      <c r="ED50" s="24"/>
+      <c r="EE50" s="24"/>
+      <c r="EF50" s="24"/>
+      <c r="EM50" s="25"/>
+      <c r="EN50" s="25"/>
+      <c r="EO50" s="25"/>
+      <c r="EP50" s="25"/>
+      <c r="EQ50" s="25"/>
+      <c r="ER50" s="25"/>
     </row>
     <row r="51" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
@@ -4664,8 +4670,8 @@
       <c r="DO51" s="8">
         <v>3</v>
       </c>
-      <c r="DP51" s="8">
-        <v>3</v>
+      <c r="DP51" s="22">
+        <v>16</v>
       </c>
       <c r="DQ51" s="9">
         <v>0</v>
@@ -4676,8 +4682,8 @@
       <c r="DS51" s="9">
         <v>0</v>
       </c>
-      <c r="DT51" s="8">
-        <v>3</v>
+      <c r="DT51" s="17">
+        <v>8</v>
       </c>
       <c r="DU51" s="8">
         <v>3</v>
@@ -4691,19 +4697,19 @@
       <c r="EA51" s="16">
         <v>7</v>
       </c>
-      <c r="EB51" s="25" t="s">
+      <c r="EB51" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="EC51" s="25"/>
-      <c r="ED51" s="25"/>
-      <c r="EE51" s="25"/>
-      <c r="EF51" s="25"/>
-      <c r="EM51" s="24"/>
-      <c r="EN51" s="24"/>
-      <c r="EO51" s="24"/>
-      <c r="EP51" s="24"/>
-      <c r="EQ51" s="24"/>
-      <c r="ER51" s="24"/>
+      <c r="EC51" s="24"/>
+      <c r="ED51" s="24"/>
+      <c r="EE51" s="24"/>
+      <c r="EF51" s="24"/>
+      <c r="EM51" s="25"/>
+      <c r="EN51" s="25"/>
+      <c r="EO51" s="25"/>
+      <c r="EP51" s="25"/>
+      <c r="EQ51" s="25"/>
+      <c r="ER51" s="25"/>
     </row>
     <row r="52" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
@@ -4828,8 +4834,8 @@
       <c r="DF52" s="9">
         <v>0</v>
       </c>
-      <c r="DG52" s="8">
-        <v>3</v>
+      <c r="DG52" s="21">
+        <v>12</v>
       </c>
       <c r="DH52" s="9">
         <v>0</v>
@@ -4837,8 +4843,8 @@
       <c r="DI52" s="9">
         <v>0</v>
       </c>
-      <c r="DJ52" s="8">
-        <v>3</v>
+      <c r="DJ52" s="21">
+        <v>12</v>
       </c>
       <c r="DK52" s="9">
         <v>0</v>
@@ -4855,8 +4861,8 @@
       <c r="DO52" s="8">
         <v>3</v>
       </c>
-      <c r="DP52" s="8">
-        <v>3</v>
+      <c r="DP52" s="21">
+        <v>12</v>
       </c>
       <c r="DQ52" s="9">
         <v>0</v>
@@ -4867,8 +4873,8 @@
       <c r="DS52" s="9">
         <v>0</v>
       </c>
-      <c r="DT52" s="8">
-        <v>3</v>
+      <c r="DT52" s="21">
+        <v>12</v>
       </c>
       <c r="DU52" s="8">
         <v>3</v>
@@ -4882,19 +4888,19 @@
       <c r="EA52" s="17">
         <v>8</v>
       </c>
-      <c r="EB52" s="25" t="s">
+      <c r="EB52" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="EC52" s="25"/>
-      <c r="ED52" s="25"/>
-      <c r="EE52" s="25"/>
-      <c r="EF52" s="25"/>
-      <c r="EM52" s="24"/>
-      <c r="EN52" s="24"/>
-      <c r="EO52" s="24"/>
-      <c r="EP52" s="24"/>
-      <c r="EQ52" s="24"/>
-      <c r="ER52" s="24"/>
+      <c r="EC52" s="24"/>
+      <c r="ED52" s="24"/>
+      <c r="EE52" s="24"/>
+      <c r="EF52" s="24"/>
+      <c r="EM52" s="25"/>
+      <c r="EN52" s="25"/>
+      <c r="EO52" s="25"/>
+      <c r="EP52" s="25"/>
+      <c r="EQ52" s="25"/>
+      <c r="ER52" s="25"/>
     </row>
     <row r="53" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -4972,20 +4978,20 @@
       <c r="CN53" s="8">
         <v>3</v>
       </c>
-      <c r="CO53" s="8">
-        <v>3</v>
+      <c r="CO53" s="20">
+        <v>11</v>
       </c>
       <c r="CP53" s="8">
         <v>3</v>
       </c>
-      <c r="CQ53" s="8">
-        <v>3</v>
+      <c r="CQ53" s="20">
+        <v>11</v>
       </c>
       <c r="CR53" s="8">
         <v>3</v>
       </c>
-      <c r="CS53" s="8">
-        <v>3</v>
+      <c r="CS53" s="22">
+        <v>13</v>
       </c>
       <c r="CT53" s="9">
         <v>0</v>
@@ -5011,8 +5017,8 @@
       <c r="DA53" s="9">
         <v>0</v>
       </c>
-      <c r="DB53" s="8">
-        <v>3</v>
+      <c r="DB53" s="22">
+        <v>13</v>
       </c>
       <c r="DC53" s="8">
         <v>3</v>
@@ -5020,14 +5026,14 @@
       <c r="DD53" s="8">
         <v>3</v>
       </c>
-      <c r="DE53" s="8">
-        <v>3</v>
+      <c r="DE53" s="22">
+        <v>16</v>
       </c>
       <c r="DF53" s="9">
         <v>0</v>
       </c>
-      <c r="DG53" s="8">
-        <v>3</v>
+      <c r="DG53" s="21">
+        <v>12</v>
       </c>
       <c r="DH53" s="9">
         <v>0</v>
@@ -5035,8 +5041,8 @@
       <c r="DI53" s="9">
         <v>0</v>
       </c>
-      <c r="DJ53" s="8">
-        <v>3</v>
+      <c r="DJ53" s="21">
+        <v>12</v>
       </c>
       <c r="DK53" s="9">
         <v>0</v>
@@ -5080,19 +5086,19 @@
       <c r="EA53" s="18">
         <v>9</v>
       </c>
-      <c r="EB53" s="25" t="s">
+      <c r="EB53" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="EC53" s="25"/>
-      <c r="ED53" s="25"/>
-      <c r="EE53" s="25"/>
-      <c r="EF53" s="25"/>
-      <c r="EM53" s="24"/>
-      <c r="EN53" s="24"/>
-      <c r="EO53" s="24"/>
-      <c r="EP53" s="24"/>
-      <c r="EQ53" s="24"/>
-      <c r="ER53" s="24"/>
+      <c r="EC53" s="24"/>
+      <c r="ED53" s="24"/>
+      <c r="EE53" s="24"/>
+      <c r="EF53" s="24"/>
+      <c r="EM53" s="25"/>
+      <c r="EN53" s="25"/>
+      <c r="EO53" s="25"/>
+      <c r="EP53" s="25"/>
+      <c r="EQ53" s="25"/>
+      <c r="ER53" s="25"/>
     </row>
     <row r="54" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
@@ -5183,8 +5189,8 @@
       <c r="CR54" s="9">
         <v>0</v>
       </c>
-      <c r="CS54" s="8">
-        <v>3</v>
+      <c r="CS54" s="20">
+        <v>11</v>
       </c>
       <c r="CT54" s="9">
         <v>0</v>
@@ -5243,14 +5249,14 @@
       <c r="DL54" s="8">
         <v>3</v>
       </c>
-      <c r="DM54" s="8">
-        <v>3</v>
-      </c>
-      <c r="DN54" s="8">
-        <v>3</v>
-      </c>
-      <c r="DO54" s="8">
-        <v>3</v>
+      <c r="DM54" s="22">
+        <v>17</v>
+      </c>
+      <c r="DN54" s="22">
+        <v>17</v>
+      </c>
+      <c r="DO54" s="22">
+        <v>16</v>
       </c>
       <c r="DP54" s="8">
         <v>3</v>
@@ -5279,19 +5285,19 @@
       <c r="EA54" s="19">
         <v>10</v>
       </c>
-      <c r="EB54" s="25" t="s">
+      <c r="EB54" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="EC54" s="25"/>
-      <c r="ED54" s="25"/>
-      <c r="EE54" s="25"/>
-      <c r="EF54" s="25"/>
-      <c r="EM54" s="24"/>
-      <c r="EN54" s="24"/>
-      <c r="EO54" s="24"/>
-      <c r="EP54" s="24"/>
-      <c r="EQ54" s="24"/>
-      <c r="ER54" s="24"/>
+      <c r="EC54" s="24"/>
+      <c r="ED54" s="24"/>
+      <c r="EE54" s="24"/>
+      <c r="EF54" s="24"/>
+      <c r="EM54" s="25"/>
+      <c r="EN54" s="25"/>
+      <c r="EO54" s="25"/>
+      <c r="EP54" s="25"/>
+      <c r="EQ54" s="25"/>
+      <c r="ER54" s="25"/>
     </row>
     <row r="55" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
@@ -5406,14 +5412,14 @@
       <c r="DA55" s="9">
         <v>0</v>
       </c>
-      <c r="DB55" s="8">
-        <v>3</v>
+      <c r="DB55" s="20">
+        <v>11</v>
       </c>
       <c r="DC55" s="8">
         <v>3</v>
       </c>
-      <c r="DD55" s="8">
-        <v>3</v>
+      <c r="DD55" s="17">
+        <v>8</v>
       </c>
       <c r="DE55" s="8">
         <v>3</v>
@@ -5436,8 +5442,8 @@
       <c r="DK55" s="8">
         <v>3</v>
       </c>
-      <c r="DL55" s="8">
-        <v>3</v>
+      <c r="DL55" s="22">
+        <v>17</v>
       </c>
       <c r="DM55" s="9">
         <v>0</v>
@@ -5460,8 +5466,8 @@
       <c r="DS55" s="9">
         <v>0</v>
       </c>
-      <c r="DT55" s="8">
-        <v>3</v>
+      <c r="DT55" s="17">
+        <v>8</v>
       </c>
       <c r="DU55" s="8">
         <v>3</v>
@@ -5475,19 +5481,19 @@
       <c r="EA55" s="20">
         <v>11</v>
       </c>
-      <c r="EB55" s="25" t="s">
+      <c r="EB55" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="EC55" s="25"/>
-      <c r="ED55" s="25"/>
-      <c r="EE55" s="25"/>
-      <c r="EF55" s="25"/>
-      <c r="EM55" s="24"/>
-      <c r="EN55" s="24"/>
-      <c r="EO55" s="24"/>
-      <c r="EP55" s="24"/>
-      <c r="EQ55" s="24"/>
-      <c r="ER55" s="24"/>
+      <c r="EC55" s="24"/>
+      <c r="ED55" s="24"/>
+      <c r="EE55" s="24"/>
+      <c r="EF55" s="24"/>
+      <c r="EM55" s="25"/>
+      <c r="EN55" s="25"/>
+      <c r="EO55" s="25"/>
+      <c r="EP55" s="25"/>
+      <c r="EQ55" s="25"/>
+      <c r="ER55" s="25"/>
     </row>
     <row r="56" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
@@ -5568,8 +5574,8 @@
       <c r="CN56" s="8">
         <v>3</v>
       </c>
-      <c r="CO56" s="8">
-        <v>3</v>
+      <c r="CO56" s="22">
+        <v>16</v>
       </c>
       <c r="CP56" s="8">
         <v>3</v>
@@ -5637,8 +5643,8 @@
       <c r="DK56" s="9">
         <v>0</v>
       </c>
-      <c r="DL56" s="8">
-        <v>3</v>
+      <c r="DL56" s="22">
+        <v>17</v>
       </c>
       <c r="DM56" s="9">
         <v>0</v>
@@ -5676,19 +5682,19 @@
       <c r="EA56" s="21">
         <v>12</v>
       </c>
-      <c r="EB56" s="25" t="s">
+      <c r="EB56" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="EC56" s="25"/>
-      <c r="ED56" s="25"/>
-      <c r="EE56" s="25"/>
-      <c r="EF56" s="25"/>
-      <c r="EM56" s="24"/>
-      <c r="EN56" s="24"/>
-      <c r="EO56" s="24"/>
-      <c r="EP56" s="24"/>
-      <c r="EQ56" s="24"/>
-      <c r="ER56" s="24"/>
+      <c r="EC56" s="24"/>
+      <c r="ED56" s="24"/>
+      <c r="EE56" s="24"/>
+      <c r="EF56" s="24"/>
+      <c r="EM56" s="25"/>
+      <c r="EN56" s="25"/>
+      <c r="EO56" s="25"/>
+      <c r="EP56" s="25"/>
+      <c r="EQ56" s="25"/>
+      <c r="ER56" s="25"/>
     </row>
     <row r="57" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
@@ -5798,8 +5804,8 @@
       <c r="DA57" s="9">
         <v>0</v>
       </c>
-      <c r="DB57" s="8">
-        <v>3</v>
+      <c r="DB57" s="20">
+        <v>11</v>
       </c>
       <c r="DC57" s="8">
         <v>3</v>
@@ -5831,14 +5837,14 @@
       <c r="DL57" s="8">
         <v>3</v>
       </c>
-      <c r="DM57" s="8">
-        <v>3</v>
-      </c>
-      <c r="DN57" s="8">
-        <v>3</v>
-      </c>
-      <c r="DO57" s="8">
-        <v>3</v>
+      <c r="DM57" s="22">
+        <v>17</v>
+      </c>
+      <c r="DN57" s="22">
+        <v>17</v>
+      </c>
+      <c r="DO57" s="22">
+        <v>17</v>
       </c>
       <c r="DP57" s="8">
         <v>3</v>
@@ -5867,22 +5873,22 @@
       <c r="EA57" s="22">
         <v>13</v>
       </c>
-      <c r="EB57" s="25" t="s">
+      <c r="EB57" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="EC57" s="25"/>
-      <c r="ED57" s="25"/>
-      <c r="EE57" s="25"/>
-      <c r="EF57" s="25"/>
-      <c r="EG57" s="25"/>
-      <c r="EH57" s="25"/>
-      <c r="EI57" s="25"/>
-      <c r="EM57" s="24"/>
-      <c r="EN57" s="24"/>
-      <c r="EO57" s="24"/>
-      <c r="EP57" s="24"/>
-      <c r="EQ57" s="24"/>
-      <c r="ER57" s="24"/>
+      <c r="EC57" s="24"/>
+      <c r="ED57" s="24"/>
+      <c r="EE57" s="24"/>
+      <c r="EF57" s="24"/>
+      <c r="EG57" s="24"/>
+      <c r="EH57" s="24"/>
+      <c r="EI57" s="24"/>
+      <c r="EM57" s="25"/>
+      <c r="EN57" s="25"/>
+      <c r="EO57" s="25"/>
+      <c r="EP57" s="25"/>
+      <c r="EQ57" s="25"/>
+      <c r="ER57" s="25"/>
     </row>
     <row r="58" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
@@ -5934,8 +5940,8 @@
       <c r="CO58" s="19">
         <v>15</v>
       </c>
-      <c r="CP58" s="8">
-        <v>3</v>
+      <c r="CP58" s="15">
+        <v>6</v>
       </c>
       <c r="CQ58" s="9">
         <v>0</v>
@@ -6036,6 +6042,16 @@
       <c r="DW58" s="14">
         <v>22</v>
       </c>
+      <c r="EA58" s="22">
+        <v>16</v>
+      </c>
+      <c r="EB58" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="EC58" s="24"/>
+      <c r="ED58" s="24"/>
+      <c r="EE58" s="24"/>
+      <c r="EF58" s="24"/>
       <c r="EM58" s="23"/>
       <c r="EN58" s="23"/>
       <c r="EO58" s="23"/>
@@ -6125,8 +6141,8 @@
       <c r="CZ59" s="8">
         <v>3</v>
       </c>
-      <c r="DA59" s="8">
-        <v>3</v>
+      <c r="DA59" s="20">
+        <v>11</v>
       </c>
       <c r="DB59" s="8">
         <v>3</v>
@@ -6179,8 +6195,8 @@
       <c r="DR59" s="9">
         <v>0</v>
       </c>
-      <c r="DS59" s="8">
-        <v>3</v>
+      <c r="DS59" s="20">
+        <v>11</v>
       </c>
       <c r="DT59" s="8">
         <v>3</v>
@@ -6194,16 +6210,19 @@
       <c r="DW59" s="14">
         <v>23</v>
       </c>
-      <c r="EA59" s="19">
-        <v>14</v>
-      </c>
-      <c r="EB59" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="EC59" s="25"/>
-      <c r="ED59" s="25"/>
-      <c r="EE59" s="25"/>
-      <c r="EF59" s="25"/>
+      <c r="EA59" s="22">
+        <v>17</v>
+      </c>
+      <c r="EB59" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="EC59" s="24"/>
+      <c r="ED59" s="24"/>
+      <c r="EE59" s="24"/>
+      <c r="EF59" s="24"/>
+      <c r="EG59" s="24"/>
+      <c r="EH59" s="24"/>
+      <c r="EI59" s="24"/>
       <c r="EM59" s="23"/>
       <c r="EN59" s="23"/>
       <c r="EO59" s="23"/>
@@ -6269,11 +6288,11 @@
       <c r="CP60" s="8">
         <v>3</v>
       </c>
-      <c r="CQ60" s="8">
-        <v>3</v>
-      </c>
-      <c r="CR60" s="8">
-        <v>3</v>
+      <c r="CQ60" s="21">
+        <v>12</v>
+      </c>
+      <c r="CR60" s="21">
+        <v>12</v>
       </c>
       <c r="CS60" s="8">
         <v>3</v>
@@ -6281,11 +6300,11 @@
       <c r="CT60" s="8">
         <v>3</v>
       </c>
-      <c r="CU60" s="8">
-        <v>3</v>
-      </c>
-      <c r="CV60" s="8">
-        <v>3</v>
+      <c r="CU60" s="16">
+        <v>7</v>
+      </c>
+      <c r="CV60" s="22">
+        <v>16</v>
       </c>
       <c r="CW60" s="8">
         <v>3</v>
@@ -6293,8 +6312,8 @@
       <c r="CX60" s="8">
         <v>3</v>
       </c>
-      <c r="CY60" s="8">
-        <v>3</v>
+      <c r="CY60" s="22">
+        <v>13</v>
       </c>
       <c r="CZ60" s="8">
         <v>3</v>
@@ -6338,11 +6357,11 @@
       <c r="DM60" s="9">
         <v>0</v>
       </c>
-      <c r="DN60" s="8">
-        <v>3</v>
-      </c>
-      <c r="DO60" s="8">
-        <v>3</v>
+      <c r="DN60" s="21">
+        <v>12</v>
+      </c>
+      <c r="DO60" s="21">
+        <v>12</v>
       </c>
       <c r="DP60" s="9">
         <v>0</v>
@@ -6368,20 +6387,6 @@
       <c r="DW60" s="14">
         <v>24</v>
       </c>
-      <c r="EA60" s="19">
-        <v>15</v>
-      </c>
-      <c r="EB60" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="EC60" s="25"/>
-      <c r="ED60" s="25"/>
-      <c r="EE60" s="25"/>
-      <c r="EF60" s="25"/>
-      <c r="EG60" s="25"/>
-      <c r="EH60" s="25"/>
-      <c r="EI60" s="25"/>
-      <c r="EJ60" s="25"/>
     </row>
     <row r="61" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
@@ -6498,8 +6503,8 @@
       <c r="DB61" s="8">
         <v>3</v>
       </c>
-      <c r="DC61" s="8">
-        <v>3</v>
+      <c r="DC61" s="17">
+        <v>8</v>
       </c>
       <c r="DD61" s="9">
         <v>0</v>
@@ -6679,32 +6684,32 @@
       <c r="DF62" s="8">
         <v>3</v>
       </c>
-      <c r="DG62" s="8">
-        <v>3</v>
+      <c r="DG62" s="20">
+        <v>11</v>
       </c>
       <c r="DH62" s="8">
         <v>3</v>
       </c>
-      <c r="DI62" s="8">
-        <v>3</v>
+      <c r="DI62" s="22">
+        <v>13</v>
       </c>
       <c r="DJ62" s="8">
         <v>3</v>
       </c>
-      <c r="DK62" s="8">
-        <v>3</v>
-      </c>
-      <c r="DL62" s="8">
-        <v>3</v>
-      </c>
-      <c r="DM62" s="8">
-        <v>3</v>
+      <c r="DK62" s="20">
+        <v>11</v>
+      </c>
+      <c r="DL62" s="22">
+        <v>16</v>
+      </c>
+      <c r="DM62" s="20">
+        <v>11</v>
       </c>
       <c r="DN62" s="8">
         <v>3</v>
       </c>
-      <c r="DO62" s="8">
-        <v>3</v>
+      <c r="DO62" s="20">
+        <v>11</v>
       </c>
       <c r="DP62" s="8">
         <v>3</v>
@@ -6730,6 +6735,16 @@
       <c r="DW62" s="14">
         <v>26</v>
       </c>
+      <c r="EA62" s="19">
+        <v>14</v>
+      </c>
+      <c r="EB62" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="EC62" s="24"/>
+      <c r="ED62" s="24"/>
+      <c r="EE62" s="24"/>
+      <c r="EF62" s="24"/>
     </row>
     <row r="63" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
@@ -6888,6 +6903,20 @@
       <c r="DW63" s="14">
         <v>27</v>
       </c>
+      <c r="EA63" s="19">
+        <v>15</v>
+      </c>
+      <c r="EB63" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="EC63" s="24"/>
+      <c r="ED63" s="24"/>
+      <c r="EE63" s="24"/>
+      <c r="EF63" s="24"/>
+      <c r="EG63" s="24"/>
+      <c r="EH63" s="24"/>
+      <c r="EI63" s="24"/>
+      <c r="EJ63" s="24"/>
     </row>
     <row r="64" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
@@ -15627,96 +15656,110 @@
       <c r="AC120">
         <v>0</v>
       </c>
-      <c r="AD120" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE120" s="25"/>
-      <c r="AF120" s="25"/>
-      <c r="AG120" s="25"/>
-      <c r="AH120" s="25"/>
+      <c r="AD120" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE120" s="24"/>
+      <c r="AF120" s="24"/>
+      <c r="AG120" s="24"/>
+      <c r="AH120" s="24"/>
     </row>
     <row r="121" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC121">
         <v>1</v>
       </c>
-      <c r="AD121" s="25" t="s">
+      <c r="AD121" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AE121" s="25"/>
-      <c r="AF121" s="25"/>
-      <c r="AG121" s="25"/>
-      <c r="AH121" s="25"/>
+      <c r="AE121" s="24"/>
+      <c r="AF121" s="24"/>
+      <c r="AG121" s="24"/>
+      <c r="AH121" s="24"/>
     </row>
     <row r="122" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC122">
         <v>2</v>
       </c>
-      <c r="AD122" s="25" t="s">
+      <c r="AD122" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AE122" s="25"/>
-      <c r="AF122" s="25"/>
-      <c r="AG122" s="25"/>
-      <c r="AH122" s="25"/>
+      <c r="AE122" s="24"/>
+      <c r="AF122" s="24"/>
+      <c r="AG122" s="24"/>
+      <c r="AH122" s="24"/>
     </row>
     <row r="123" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC123">
         <v>3</v>
       </c>
-      <c r="AD123" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE123" s="25"/>
-      <c r="AF123" s="25"/>
-      <c r="AG123" s="25"/>
-      <c r="AH123" s="25"/>
+      <c r="AD123" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE123" s="24"/>
+      <c r="AF123" s="24"/>
+      <c r="AG123" s="24"/>
+      <c r="AH123" s="24"/>
     </row>
     <row r="124" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC124">
         <v>4</v>
       </c>
-      <c r="AD124" s="25" t="s">
+      <c r="AD124" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AE124" s="25"/>
-      <c r="AF124" s="25"/>
-      <c r="AG124" s="25"/>
-      <c r="AH124" s="25"/>
+      <c r="AE124" s="24"/>
+      <c r="AF124" s="24"/>
+      <c r="AG124" s="24"/>
+      <c r="AH124" s="24"/>
     </row>
     <row r="125" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC125">
         <v>5</v>
       </c>
-      <c r="AD125" s="25" t="s">
+      <c r="AD125" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AE125" s="25"/>
-      <c r="AF125" s="25"/>
-      <c r="AG125" s="25"/>
-      <c r="AH125" s="25"/>
+      <c r="AE125" s="24"/>
+      <c r="AF125" s="24"/>
+      <c r="AG125" s="24"/>
+      <c r="AH125" s="24"/>
     </row>
     <row r="126" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC126">
         <v>6</v>
       </c>
-      <c r="AD126" s="25" t="s">
+      <c r="AD126" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AE126" s="25"/>
-      <c r="AF126" s="25"/>
-      <c r="AG126" s="25"/>
-      <c r="AH126" s="25"/>
+      <c r="AE126" s="24"/>
+      <c r="AF126" s="24"/>
+      <c r="AG126" s="24"/>
+      <c r="AH126" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="EB49:EF49"/>
-    <mergeCell ref="EB50:EF50"/>
-    <mergeCell ref="EB51:EF51"/>
-    <mergeCell ref="EB44:EF44"/>
-    <mergeCell ref="EB45:EF45"/>
-    <mergeCell ref="EB46:EF46"/>
-    <mergeCell ref="EB47:EF47"/>
-    <mergeCell ref="EB48:EF48"/>
+  <mergeCells count="46">
+    <mergeCell ref="EB59:EI59"/>
+    <mergeCell ref="EM47:ER47"/>
+    <mergeCell ref="EM48:EO48"/>
+    <mergeCell ref="EP48:ER48"/>
+    <mergeCell ref="EM49:EO49"/>
+    <mergeCell ref="EM50:EO50"/>
+    <mergeCell ref="EM56:EO56"/>
+    <mergeCell ref="EM57:EO57"/>
+    <mergeCell ref="EP49:ER49"/>
+    <mergeCell ref="EP50:ER50"/>
+    <mergeCell ref="EP51:ER51"/>
+    <mergeCell ref="EM51:EO51"/>
+    <mergeCell ref="EM52:EO52"/>
+    <mergeCell ref="EM53:EO53"/>
+    <mergeCell ref="EM54:EO54"/>
+    <mergeCell ref="EM55:EO55"/>
+    <mergeCell ref="EP57:ER57"/>
+    <mergeCell ref="EP52:ER52"/>
+    <mergeCell ref="EP53:ER53"/>
+    <mergeCell ref="EP54:ER54"/>
+    <mergeCell ref="EP55:ER55"/>
+    <mergeCell ref="EP56:ER56"/>
     <mergeCell ref="EB52:EF52"/>
     <mergeCell ref="EB53:EF53"/>
     <mergeCell ref="EB54:EF54"/>
@@ -15727,32 +15770,20 @@
     <mergeCell ref="AD123:AH123"/>
     <mergeCell ref="AD124:AH124"/>
     <mergeCell ref="AD125:AH125"/>
-    <mergeCell ref="EB59:EF59"/>
+    <mergeCell ref="EB62:EF62"/>
     <mergeCell ref="EB55:EF55"/>
     <mergeCell ref="EB56:EF56"/>
     <mergeCell ref="EB57:EI57"/>
-    <mergeCell ref="EB60:EJ60"/>
-    <mergeCell ref="EM56:EO56"/>
-    <mergeCell ref="EM57:EO57"/>
-    <mergeCell ref="EP49:ER49"/>
-    <mergeCell ref="EP50:ER50"/>
-    <mergeCell ref="EP51:ER51"/>
-    <mergeCell ref="EM51:EO51"/>
-    <mergeCell ref="EM52:EO52"/>
-    <mergeCell ref="EM53:EO53"/>
-    <mergeCell ref="EM54:EO54"/>
-    <mergeCell ref="EM55:EO55"/>
-    <mergeCell ref="EM47:ER47"/>
-    <mergeCell ref="EM48:EO48"/>
-    <mergeCell ref="EP48:ER48"/>
-    <mergeCell ref="EM49:EO49"/>
-    <mergeCell ref="EM50:EO50"/>
-    <mergeCell ref="EP57:ER57"/>
-    <mergeCell ref="EP52:ER52"/>
-    <mergeCell ref="EP53:ER53"/>
-    <mergeCell ref="EP54:ER54"/>
-    <mergeCell ref="EP55:ER55"/>
-    <mergeCell ref="EP56:ER56"/>
+    <mergeCell ref="EB63:EJ63"/>
+    <mergeCell ref="EB58:EF58"/>
+    <mergeCell ref="EB49:EF49"/>
+    <mergeCell ref="EB50:EF50"/>
+    <mergeCell ref="EB51:EF51"/>
+    <mergeCell ref="EB44:EF44"/>
+    <mergeCell ref="EB45:EF45"/>
+    <mergeCell ref="EB46:EF46"/>
+    <mergeCell ref="EB47:EF47"/>
+    <mergeCell ref="EB48:EF48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
My worst fear is i dont even know what i just did
</commit_message>
<xml_diff>
--- a/documents/Map/Map.xlsx
+++ b/documents/Map/Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tk-hdd-backup\Data\@KMUTNB WORKs\JavaGameProject\documents\Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athicha/Desktop/JavaGameProject/documents/Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930892AB-AECB-4A94-95EA-1EFD429D8E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA44807A-7700-1B4C-972F-3299C668DD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{ADFB26D6-5F36-0045-9469-D0CB3B23D93E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,16 +709,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84092400-AD61-BC4A-9F6E-C24F40418E60}">
   <dimension ref="B2:ES126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EM51" sqref="EM51:EO51"/>
+    <sheetView tabSelected="1" topLeftCell="BP32" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="DQ38" sqref="DQ38:DT43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="83" max="83" width="2.625" customWidth="1"/>
+    <col min="83" max="83" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -734,16 +734,16 @@
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
     </row>
-    <row r="3" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AM3" s="1"/>
     </row>
-    <row r="4" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z4" s="1"/>
       <c r="AM4" s="1"/>
     </row>
-    <row r="5" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z5" s="1"/>
       <c r="AM5" s="1"/>
       <c r="CW5" s="1"/>
@@ -755,7 +755,7 @@
       <c r="DC5" s="1"/>
       <c r="DD5" s="1"/>
     </row>
-    <row r="6" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AM6" s="1"/>
@@ -763,7 +763,7 @@
       <c r="CZ6" s="1"/>
       <c r="DD6" s="1"/>
     </row>
-    <row r="7" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -804,7 +804,7 @@
       <c r="CW7" s="1"/>
       <c r="DD7" s="1"/>
     </row>
-    <row r="8" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AD8" s="1"/>
@@ -813,7 +813,7 @@
       <c r="CW8" s="1"/>
       <c r="DD8" s="1"/>
     </row>
-    <row r="9" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AD9" s="1"/>
@@ -829,7 +829,7 @@
       <c r="DG9" s="1"/>
       <c r="DH9" s="1"/>
     </row>
-    <row r="10" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R10" s="1"/>
       <c r="V10" s="1"/>
       <c r="Z10" s="1"/>
@@ -868,7 +868,7 @@
       <c r="CZ10" s="1"/>
       <c r="DH10" s="1"/>
     </row>
-    <row r="11" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AM11" s="1"/>
@@ -892,7 +892,7 @@
       <c r="DM11" s="1"/>
       <c r="DN11" s="1"/>
     </row>
-    <row r="12" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AM12" s="1"/>
@@ -911,7 +911,7 @@
       <c r="DL12" s="13"/>
       <c r="DN12" s="1"/>
     </row>
-    <row r="13" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R13" s="1"/>
       <c r="V13" s="1"/>
       <c r="Z13" s="1"/>
@@ -928,7 +928,7 @@
       <c r="DE13" s="1"/>
       <c r="DN13" s="1"/>
     </row>
-    <row r="14" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AM14" s="1"/>
@@ -958,7 +958,7 @@
       <c r="DK14" s="13"/>
       <c r="DN14" s="1"/>
     </row>
-    <row r="15" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5"/>
@@ -993,7 +993,7 @@
       <c r="DE15" s="1"/>
       <c r="DN15" s="1"/>
     </row>
-    <row r="16" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="1"/>
       <c r="J16" s="1"/>
       <c r="R16" s="1"/>
@@ -1013,7 +1013,7 @@
       <c r="DL16" s="1"/>
       <c r="DN16" s="1"/>
     </row>
-    <row r="17" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1072,7 +1072,7 @@
       <c r="DU17" s="1"/>
       <c r="DV17" s="1"/>
     </row>
-    <row r="18" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E18" s="1"/>
       <c r="U18" s="1"/>
       <c r="Z18" s="1"/>
@@ -1116,7 +1116,7 @@
       <c r="DP18" s="1"/>
       <c r="DV18" s="1"/>
     </row>
-    <row r="19" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="1"/>
       <c r="U19" s="1"/>
       <c r="AJ19" s="1"/>
@@ -1148,7 +1148,7 @@
       <c r="DU19" s="1"/>
       <c r="DV19" s="1"/>
     </row>
-    <row r="20" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="1"/>
       <c r="U20" s="1"/>
       <c r="AJ20" s="1"/>
@@ -1172,7 +1172,7 @@
       <c r="DP20" s="1"/>
       <c r="DT20" s="1"/>
     </row>
-    <row r="21" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="1"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1200,7 +1200,7 @@
       <c r="DP21" s="1"/>
       <c r="DT21" s="1"/>
     </row>
-    <row r="22" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E22" s="1"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1252,7 +1252,7 @@
       <c r="DS22" s="1"/>
       <c r="DT22" s="1"/>
     </row>
-    <row r="23" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1286,7 +1286,7 @@
       <c r="DP23" s="1"/>
       <c r="DT23" s="1"/>
     </row>
-    <row r="24" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E24" s="1"/>
       <c r="J24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1314,7 +1314,7 @@
       <c r="DL24" s="1"/>
       <c r="DT24" s="1"/>
     </row>
-    <row r="25" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E25" s="1"/>
       <c r="J25" s="1"/>
       <c r="Q25" s="1"/>
@@ -1340,7 +1340,7 @@
       <c r="DP25" s="1"/>
       <c r="DT25" s="1"/>
     </row>
-    <row r="26" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="Z26" s="5"/>
@@ -1375,7 +1375,7 @@
       <c r="DS26" s="1"/>
       <c r="DT26" s="1"/>
     </row>
-    <row r="27" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="U27" s="1"/>
@@ -1410,7 +1410,7 @@
       <c r="DL27" s="1"/>
       <c r="DS27" s="1"/>
     </row>
-    <row r="28" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E28" s="1"/>
       <c r="J28" s="1"/>
       <c r="Q28" s="1"/>
@@ -1431,7 +1431,7 @@
       <c r="DL28" s="1"/>
       <c r="DS28" s="1"/>
     </row>
-    <row r="29" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E29" s="1"/>
       <c r="J29" s="1"/>
       <c r="Q29" s="1"/>
@@ -1484,7 +1484,7 @@
       <c r="DR29" s="1"/>
       <c r="DS29" s="1"/>
     </row>
-    <row r="30" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="I30" s="1"/>
@@ -1522,7 +1522,7 @@
       <c r="DE30" s="1"/>
       <c r="DQ30" s="1"/>
     </row>
-    <row r="31" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="Y31" s="1"/>
@@ -1550,7 +1550,7 @@
       <c r="DP31" s="1"/>
       <c r="DQ31" s="1"/>
     </row>
-    <row r="32" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1584,7 +1584,7 @@
       <c r="CH32" s="1"/>
       <c r="CQ32" s="1"/>
     </row>
-    <row r="33" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="Y33" s="1"/>
@@ -1602,7 +1602,7 @@
       <c r="CP33" s="1"/>
       <c r="CQ33" s="1"/>
     </row>
-    <row r="34" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
       <c r="I34" s="3"/>
@@ -1618,7 +1618,7 @@
       <c r="AP34" s="1"/>
       <c r="BK34" s="1"/>
     </row>
-    <row r="35" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="Y35" s="1"/>
@@ -1755,7 +1755,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="Y37" s="1"/>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2222,7 +2222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="CE39" s="14">
         <v>3</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="CE40" s="14">
         <v>4</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2704,7 +2704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2901,7 +2901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -3097,7 +3097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3303,7 +3303,7 @@
       <c r="EE44" s="24"/>
       <c r="EF44" s="24"/>
     </row>
-    <row r="45" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3510,7 +3510,7 @@
       <c r="EE45" s="24"/>
       <c r="EF45" s="24"/>
     </row>
-    <row r="46" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3723,7 +3723,7 @@
       <c r="EE46" s="24"/>
       <c r="EF46" s="24"/>
     </row>
-    <row r="47" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3917,7 +3917,7 @@
       <c r="EQ47" s="25"/>
       <c r="ER47" s="25"/>
     </row>
-    <row r="48" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -4113,7 +4113,7 @@
       <c r="EQ48" s="25"/>
       <c r="ER48" s="25"/>
     </row>
-    <row r="49" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -4332,7 +4332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -4530,7 +4530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4728,7 +4728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -4926,7 +4926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5131,7 +5131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -5337,7 +5337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5540,7 +5540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5741,7 +5741,7 @@
       <c r="EQ56" s="25"/>
       <c r="ER56" s="25"/>
     </row>
-    <row r="57" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -5935,7 +5935,7 @@
       <c r="EQ57" s="25"/>
       <c r="ER57" s="25"/>
     </row>
-    <row r="58" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -6104,7 +6104,7 @@
       <c r="EQ58" s="23"/>
       <c r="ER58" s="23"/>
     </row>
-    <row r="59" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -6275,7 +6275,7 @@
       <c r="EQ59" s="23"/>
       <c r="ER59" s="23"/>
     </row>
-    <row r="60" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -6433,7 +6433,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -6612,7 +6612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -6791,7 +6791,7 @@
       <c r="EE62" s="24"/>
       <c r="EF62" s="24"/>
     </row>
-    <row r="63" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -6963,7 +6963,7 @@
       <c r="EI63" s="24"/>
       <c r="EJ63" s="24"/>
     </row>
-    <row r="64" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -7119,7 +7119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -7269,7 +7269,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -7304,7 +7304,7 @@
       <c r="BS66" s="1"/>
       <c r="BT66" s="1"/>
     </row>
-    <row r="67" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -7326,7 +7326,7 @@
       <c r="BS67" s="1"/>
       <c r="BT67" s="1"/>
     </row>
-    <row r="68" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -7357,7 +7357,7 @@
       <c r="BS68" s="1"/>
       <c r="BT68" s="1"/>
     </row>
-    <row r="69" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -7398,7 +7398,7 @@
       <c r="BS69" s="1"/>
       <c r="BT69" s="1"/>
     </row>
-    <row r="70" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -7424,7 +7424,7 @@
       <c r="BS70" s="1"/>
       <c r="BT70" s="1"/>
     </row>
-    <row r="71" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -7468,7 +7468,7 @@
       <c r="BS71" s="1"/>
       <c r="BT71" s="1"/>
     </row>
-    <row r="72" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="R72" s="1"/>
@@ -7496,7 +7496,7 @@
       <c r="BS72" s="1"/>
       <c r="BT72" s="1"/>
     </row>
-    <row r="73" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="E73" s="2"/>
@@ -7532,7 +7532,7 @@
       <c r="BS73" s="1"/>
       <c r="BT73" s="1"/>
     </row>
-    <row r="74" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="R74" s="1"/>
@@ -7560,7 +7560,7 @@
       <c r="BS74" s="1"/>
       <c r="BT74" s="1"/>
     </row>
-    <row r="75" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -7614,7 +7614,7 @@
       <c r="BS75" s="1"/>
       <c r="BT75" s="1"/>
     </row>
-    <row r="76" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -7669,7 +7669,7 @@
       <c r="BS76" s="1"/>
       <c r="BT76" s="1"/>
     </row>
-    <row r="77" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -7742,7 +7742,7 @@
       <c r="BS77" s="1"/>
       <c r="BT77" s="1"/>
     </row>
-    <row r="79" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="8">
         <v>3</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="8">
         <v>3</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="8">
         <v>3</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="8">
         <v>3</v>
       </c>
@@ -8602,7 +8602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="8">
         <v>3</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="8">
         <v>3</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="8">
         <v>3</v>
       </c>
@@ -9247,7 +9247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="8">
         <v>3</v>
       </c>
@@ -9462,7 +9462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="8">
         <v>3</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="8">
         <v>3</v>
       </c>
@@ -9892,7 +9892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="8">
         <v>3</v>
       </c>
@@ -10107,7 +10107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="8">
         <v>3</v>
       </c>
@@ -10322,7 +10322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="8">
         <v>3</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="8">
         <v>3</v>
       </c>
@@ -10752,7 +10752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="8">
         <v>3</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="8">
         <v>3</v>
       </c>
@@ -11182,7 +11182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="8">
         <v>3</v>
       </c>
@@ -11397,7 +11397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="8">
         <v>3</v>
       </c>
@@ -11612,7 +11612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="8">
         <v>3</v>
       </c>
@@ -11827,7 +11827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="8">
         <v>3</v>
       </c>
@@ -12042,7 +12042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="8">
         <v>3</v>
       </c>
@@ -12257,7 +12257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="8">
         <v>3</v>
       </c>
@@ -12472,7 +12472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="8">
         <v>3</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="8">
         <v>3</v>
       </c>
@@ -12902,7 +12902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="8">
         <v>3</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="8">
         <v>3</v>
       </c>
@@ -13332,7 +13332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="8">
         <v>3</v>
       </c>
@@ -13547,7 +13547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="8">
         <v>3</v>
       </c>
@@ -13762,7 +13762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="8">
         <v>3</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="8">
         <v>3</v>
       </c>
@@ -14192,7 +14192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="8">
         <v>3</v>
       </c>
@@ -14407,7 +14407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="8">
         <v>3</v>
       </c>
@@ -14622,7 +14622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="8">
         <v>3</v>
       </c>
@@ -14837,7 +14837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="8">
         <v>3</v>
       </c>
@@ -15052,7 +15052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="8">
         <v>3</v>
       </c>
@@ -15267,7 +15267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="8">
         <v>3</v>
       </c>
@@ -15482,7 +15482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="8">
         <v>3</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC120">
         <v>0</v>
       </c>
@@ -15709,7 +15709,7 @@
       <c r="AG120" s="24"/>
       <c r="AH120" s="24"/>
     </row>
-    <row r="121" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC121">
         <v>1</v>
       </c>
@@ -15721,7 +15721,7 @@
       <c r="AG121" s="24"/>
       <c r="AH121" s="24"/>
     </row>
-    <row r="122" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC122">
         <v>2</v>
       </c>
@@ -15733,7 +15733,7 @@
       <c r="AG122" s="24"/>
       <c r="AH122" s="24"/>
     </row>
-    <row r="123" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC123">
         <v>3</v>
       </c>
@@ -15745,7 +15745,7 @@
       <c r="AG123" s="24"/>
       <c r="AH123" s="24"/>
     </row>
-    <row r="124" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC124">
         <v>4</v>
       </c>
@@ -15757,7 +15757,7 @@
       <c r="AG124" s="24"/>
       <c r="AH124" s="24"/>
     </row>
-    <row r="125" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC125">
         <v>5</v>
       </c>
@@ -15769,7 +15769,7 @@
       <c r="AG125" s="24"/>
       <c r="AH125" s="24"/>
     </row>
-    <row r="126" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC126">
         <v>6</v>
       </c>
@@ -15783,14 +15783,28 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="EB49:EF49"/>
-    <mergeCell ref="EB50:EF50"/>
-    <mergeCell ref="EB51:EF51"/>
-    <mergeCell ref="EB44:EF44"/>
-    <mergeCell ref="EB45:EF45"/>
-    <mergeCell ref="EB46:EF46"/>
-    <mergeCell ref="EB47:EF47"/>
-    <mergeCell ref="EB48:EF48"/>
+    <mergeCell ref="EB59:EI59"/>
+    <mergeCell ref="EM47:ER47"/>
+    <mergeCell ref="EM48:EO48"/>
+    <mergeCell ref="EP48:ER48"/>
+    <mergeCell ref="EM49:EO49"/>
+    <mergeCell ref="EM50:EO50"/>
+    <mergeCell ref="EM56:EO56"/>
+    <mergeCell ref="EM57:EO57"/>
+    <mergeCell ref="EP49:ER49"/>
+    <mergeCell ref="EP50:ER50"/>
+    <mergeCell ref="EP51:ER51"/>
+    <mergeCell ref="EM51:EO51"/>
+    <mergeCell ref="EM52:EO52"/>
+    <mergeCell ref="EM53:EO53"/>
+    <mergeCell ref="EM54:EO54"/>
+    <mergeCell ref="EM55:EO55"/>
+    <mergeCell ref="EP57:ER57"/>
+    <mergeCell ref="EP52:ER52"/>
+    <mergeCell ref="EP53:ER53"/>
+    <mergeCell ref="EP54:ER54"/>
+    <mergeCell ref="EP55:ER55"/>
+    <mergeCell ref="EP56:ER56"/>
     <mergeCell ref="EB52:EF52"/>
     <mergeCell ref="EB53:EF53"/>
     <mergeCell ref="EB54:EF54"/>
@@ -15807,28 +15821,14 @@
     <mergeCell ref="EB57:EI57"/>
     <mergeCell ref="EB63:EJ63"/>
     <mergeCell ref="EB58:EF58"/>
-    <mergeCell ref="EP57:ER57"/>
-    <mergeCell ref="EP52:ER52"/>
-    <mergeCell ref="EP53:ER53"/>
-    <mergeCell ref="EP54:ER54"/>
-    <mergeCell ref="EP55:ER55"/>
-    <mergeCell ref="EP56:ER56"/>
-    <mergeCell ref="EB59:EI59"/>
-    <mergeCell ref="EM47:ER47"/>
-    <mergeCell ref="EM48:EO48"/>
-    <mergeCell ref="EP48:ER48"/>
-    <mergeCell ref="EM49:EO49"/>
-    <mergeCell ref="EM50:EO50"/>
-    <mergeCell ref="EM56:EO56"/>
-    <mergeCell ref="EM57:EO57"/>
-    <mergeCell ref="EP49:ER49"/>
-    <mergeCell ref="EP50:ER50"/>
-    <mergeCell ref="EP51:ER51"/>
-    <mergeCell ref="EM51:EO51"/>
-    <mergeCell ref="EM52:EO52"/>
-    <mergeCell ref="EM53:EO53"/>
-    <mergeCell ref="EM54:EO54"/>
-    <mergeCell ref="EM55:EO55"/>
+    <mergeCell ref="EB49:EF49"/>
+    <mergeCell ref="EB50:EF50"/>
+    <mergeCell ref="EB51:EF51"/>
+    <mergeCell ref="EB44:EF44"/>
+    <mergeCell ref="EB45:EF45"/>
+    <mergeCell ref="EB46:EF46"/>
+    <mergeCell ref="EB47:EF47"/>
+    <mergeCell ref="EB48:EF48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
j o s h
</commit_message>
<xml_diff>
--- a/documents/Map/Map.xlsx
+++ b/documents/Map/Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athicha/Desktop/JavaGameProject/documents/Map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tk-hdd-backup\Data\@KMUTNB WORKs\JavaGameProject\documents\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B557EB0-174A-854E-B4C0-E704AC488DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636DA52B-BF47-4155-999B-D68DACC11F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,10 +335,10 @@
     <xf numFmtId="3" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -648,24 +648,24 @@
   </sheetPr>
   <dimension ref="B2:ES126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA35" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="DI48" sqref="DI48"/>
+    <sheetView tabSelected="1" topLeftCell="CA59" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="CF71" sqref="CF71:DA86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.1640625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="28" width="3.1640625" style="1"/>
-    <col min="29" max="29" width="3.1640625" style="2"/>
-    <col min="30" max="34" width="3.1640625" style="3"/>
-    <col min="35" max="72" width="3.1640625" style="1"/>
-    <col min="83" max="127" width="3.1640625" style="1"/>
-    <col min="131" max="131" width="3.1640625" style="1"/>
-    <col min="143" max="143" width="3.1640625" style="1"/>
-    <col min="146" max="146" width="3.1640625" style="1"/>
-    <col min="149" max="149" width="3.1640625" style="1"/>
+    <col min="2" max="28" width="3.140625" style="1"/>
+    <col min="29" max="29" width="3.140625" style="2"/>
+    <col min="30" max="34" width="3.140625" style="3"/>
+    <col min="35" max="72" width="3.140625" style="1"/>
+    <col min="83" max="127" width="3.140625" style="1"/>
+    <col min="131" max="131" width="3.140625" style="1"/>
+    <col min="143" max="143" width="3.140625" style="1"/>
+    <col min="146" max="146" width="3.140625" style="1"/>
+    <col min="149" max="149" width="3.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
@@ -681,16 +681,16 @@
       <c r="AL2" s="4"/>
       <c r="AM2" s="4"/>
     </row>
-    <row r="3" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z3" s="4"/>
       <c r="AD3" s="4"/>
       <c r="AM3" s="4"/>
     </row>
-    <row r="4" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z4" s="4"/>
       <c r="AM4" s="4"/>
     </row>
-    <row r="5" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="CW5" s="4"/>
@@ -702,7 +702,7 @@
       <c r="DC5" s="4"/>
       <c r="DD5" s="4"/>
     </row>
-    <row r="6" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z6" s="4"/>
       <c r="AD6" s="4"/>
       <c r="AM6" s="4"/>
@@ -710,7 +710,7 @@
       <c r="CZ6" s="4"/>
       <c r="DD6" s="4"/>
     </row>
-    <row r="7" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -751,7 +751,7 @@
       <c r="CW7" s="4"/>
       <c r="DD7" s="4"/>
     </row>
-    <row r="8" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AD8" s="4"/>
@@ -760,7 +760,7 @@
       <c r="CW8" s="4"/>
       <c r="DD8" s="4"/>
     </row>
-    <row r="9" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R9" s="4"/>
       <c r="Z9" s="4"/>
       <c r="AD9" s="4"/>
@@ -776,7 +776,7 @@
       <c r="DG9" s="4"/>
       <c r="DH9" s="4"/>
     </row>
-    <row r="10" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R10" s="4"/>
       <c r="V10" s="4"/>
       <c r="Z10" s="4"/>
@@ -815,7 +815,7 @@
       <c r="CZ10" s="4"/>
       <c r="DH10" s="4"/>
     </row>
-    <row r="11" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AM11" s="4"/>
@@ -839,7 +839,7 @@
       <c r="DM11" s="4"/>
       <c r="DN11" s="4"/>
     </row>
-    <row r="12" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AM12" s="4"/>
@@ -858,7 +858,7 @@
       <c r="DL12" s="6"/>
       <c r="DN12" s="4"/>
     </row>
-    <row r="13" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R13" s="4"/>
       <c r="V13" s="4"/>
       <c r="Z13" s="4"/>
@@ -875,7 +875,7 @@
       <c r="DE13" s="4"/>
       <c r="DN13" s="4"/>
     </row>
-    <row r="14" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R14" s="4"/>
       <c r="Z14" s="4"/>
       <c r="AM14" s="4"/>
@@ -905,7 +905,7 @@
       <c r="DK14" s="6"/>
       <c r="DN14" s="4"/>
     </row>
-    <row r="15" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
@@ -940,7 +940,7 @@
       <c r="DE15" s="4"/>
       <c r="DN15" s="4"/>
     </row>
-    <row r="16" spans="5:118" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="5:118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="J16" s="4"/>
       <c r="R16" s="4"/>
@@ -960,7 +960,7 @@
       <c r="DL16" s="4"/>
       <c r="DN16" s="4"/>
     </row>
-    <row r="17" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -1019,7 +1019,7 @@
       <c r="DU17" s="4"/>
       <c r="DV17" s="4"/>
     </row>
-    <row r="18" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="4"/>
       <c r="U18" s="4"/>
       <c r="Z18" s="4"/>
@@ -1063,7 +1063,7 @@
       <c r="DP18" s="4"/>
       <c r="DV18" s="4"/>
     </row>
-    <row r="19" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="4"/>
       <c r="U19" s="4"/>
       <c r="AJ19" s="4"/>
@@ -1095,7 +1095,7 @@
       <c r="DU19" s="4"/>
       <c r="DV19" s="4"/>
     </row>
-    <row r="20" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="4"/>
       <c r="U20" s="4"/>
       <c r="AJ20" s="4"/>
@@ -1119,7 +1119,7 @@
       <c r="DP20" s="4"/>
       <c r="DT20" s="4"/>
     </row>
-    <row r="21" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="4"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1147,7 +1147,7 @@
       <c r="DP21" s="4"/>
       <c r="DT21" s="4"/>
     </row>
-    <row r="22" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="4"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1199,7 +1199,7 @@
       <c r="DS22" s="4"/>
       <c r="DT22" s="4"/>
     </row>
-    <row r="23" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1233,7 +1233,7 @@
       <c r="DP23" s="4"/>
       <c r="DT23" s="4"/>
     </row>
-    <row r="24" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="4"/>
       <c r="J24" s="4"/>
       <c r="Q24" s="4"/>
@@ -1261,7 +1261,7 @@
       <c r="DL24" s="4"/>
       <c r="DT24" s="4"/>
     </row>
-    <row r="25" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="4"/>
       <c r="J25" s="4"/>
       <c r="Q25" s="4"/>
@@ -1287,7 +1287,7 @@
       <c r="DP25" s="4"/>
       <c r="DT25" s="4"/>
     </row>
-    <row r="26" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="Z26" s="5"/>
@@ -1322,7 +1322,7 @@
       <c r="DS26" s="4"/>
       <c r="DT26" s="4"/>
     </row>
-    <row r="27" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="U27" s="4"/>
@@ -1357,7 +1357,7 @@
       <c r="DL27" s="4"/>
       <c r="DS27" s="4"/>
     </row>
-    <row r="28" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="4"/>
       <c r="J28" s="4"/>
       <c r="Q28" s="4"/>
@@ -1378,7 +1378,7 @@
       <c r="DL28" s="4"/>
       <c r="DS28" s="4"/>
     </row>
-    <row r="29" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="4"/>
       <c r="J29" s="4"/>
       <c r="Q29" s="4"/>
@@ -1431,7 +1431,7 @@
       <c r="DR29" s="4"/>
       <c r="DS29" s="4"/>
     </row>
-    <row r="30" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="I30" s="4"/>
@@ -1469,7 +1469,7 @@
       <c r="DE30" s="4"/>
       <c r="DQ30" s="4"/>
     </row>
-    <row r="31" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="Y31" s="4"/>
@@ -1497,7 +1497,7 @@
       <c r="DP31" s="4"/>
       <c r="DQ31" s="4"/>
     </row>
-    <row r="32" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1531,7 +1531,7 @@
       <c r="CH32" s="4"/>
       <c r="CQ32" s="4"/>
     </row>
-    <row r="33" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="Y33" s="4"/>
@@ -1549,7 +1549,7 @@
       <c r="CP33" s="4"/>
       <c r="CQ33" s="4"/>
     </row>
-    <row r="34" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="D34" s="10"/>
       <c r="I34" s="11"/>
@@ -1565,7 +1565,7 @@
       <c r="AP34" s="4"/>
       <c r="BK34" s="4"/>
     </row>
-    <row r="35" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="Y35" s="4"/>
@@ -1702,7 +1702,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1871,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="Y37" s="4"/>
@@ -2011,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2169,7 +2169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CE39" s="12">
         <v>3</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CE40" s="12">
         <v>4</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -2651,7 +2651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2848,7 +2848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -3044,7 +3044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -3242,15 +3242,15 @@
       <c r="EA44" s="17">
         <v>0</v>
       </c>
-      <c r="EB44" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="EC44" s="29"/>
-      <c r="ED44" s="29"/>
-      <c r="EE44" s="29"/>
-      <c r="EF44" s="29"/>
+      <c r="EB44" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="EC44" s="28"/>
+      <c r="ED44" s="28"/>
+      <c r="EE44" s="28"/>
+      <c r="EF44" s="28"/>
     </row>
-    <row r="45" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -3449,15 +3449,15 @@
       <c r="EA45" s="17">
         <v>1</v>
       </c>
-      <c r="EB45" s="29" t="s">
+      <c r="EB45" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="EC45" s="29"/>
-      <c r="ED45" s="29"/>
-      <c r="EE45" s="29"/>
-      <c r="EF45" s="29"/>
+      <c r="EC45" s="28"/>
+      <c r="ED45" s="28"/>
+      <c r="EE45" s="28"/>
+      <c r="EF45" s="28"/>
     </row>
-    <row r="46" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -3662,15 +3662,15 @@
       <c r="EA46" s="17">
         <v>2</v>
       </c>
-      <c r="EB46" s="29" t="s">
+      <c r="EB46" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="EC46" s="29"/>
-      <c r="ED46" s="29"/>
-      <c r="EE46" s="29"/>
-      <c r="EF46" s="29"/>
+      <c r="EC46" s="28"/>
+      <c r="ED46" s="28"/>
+      <c r="EE46" s="28"/>
+      <c r="EF46" s="28"/>
     </row>
-    <row r="47" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -3848,23 +3848,23 @@
       <c r="EA47" s="13">
         <v>3</v>
       </c>
-      <c r="EB47" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="EC47" s="29"/>
-      <c r="ED47" s="29"/>
-      <c r="EE47" s="29"/>
-      <c r="EF47" s="29"/>
-      <c r="EM47" s="28" t="s">
+      <c r="EB47" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="EC47" s="28"/>
+      <c r="ED47" s="28"/>
+      <c r="EE47" s="28"/>
+      <c r="EF47" s="28"/>
+      <c r="EM47" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="EN47" s="29"/>
-      <c r="EO47" s="29"/>
-      <c r="EP47" s="28"/>
-      <c r="EQ47" s="29"/>
-      <c r="ER47" s="29"/>
+      <c r="EN47" s="28"/>
+      <c r="EO47" s="28"/>
+      <c r="EP47" s="29"/>
+      <c r="EQ47" s="28"/>
+      <c r="ER47" s="28"/>
     </row>
-    <row r="48" spans="2:148" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:148" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -4042,25 +4042,25 @@
       <c r="EA48" s="17">
         <v>4</v>
       </c>
-      <c r="EB48" s="29" t="s">
+      <c r="EB48" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="EC48" s="29"/>
-      <c r="ED48" s="29"/>
-      <c r="EE48" s="29"/>
-      <c r="EF48" s="29"/>
-      <c r="EM48" s="28" t="s">
+      <c r="EC48" s="28"/>
+      <c r="ED48" s="28"/>
+      <c r="EE48" s="28"/>
+      <c r="EF48" s="28"/>
+      <c r="EM48" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="EN48" s="29"/>
-      <c r="EO48" s="29"/>
-      <c r="EP48" s="28" t="s">
+      <c r="EN48" s="28"/>
+      <c r="EO48" s="28"/>
+      <c r="EP48" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="EQ48" s="29"/>
-      <c r="ER48" s="29"/>
+      <c r="EQ48" s="28"/>
+      <c r="ER48" s="28"/>
     </row>
-    <row r="49" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -4258,28 +4258,28 @@
       <c r="EA49" s="17">
         <v>5</v>
       </c>
-      <c r="EB49" s="29" t="s">
+      <c r="EB49" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="EC49" s="29"/>
-      <c r="ED49" s="29"/>
-      <c r="EE49" s="29"/>
-      <c r="EF49" s="29"/>
-      <c r="EM49" s="28">
+      <c r="EC49" s="28"/>
+      <c r="ED49" s="28"/>
+      <c r="EE49" s="28"/>
+      <c r="EF49" s="28"/>
+      <c r="EM49" s="29">
         <v>5</v>
       </c>
-      <c r="EN49" s="29"/>
-      <c r="EO49" s="29"/>
-      <c r="EP49" s="28">
+      <c r="EN49" s="28"/>
+      <c r="EO49" s="28"/>
+      <c r="EP49" s="29">
         <v>26</v>
       </c>
-      <c r="EQ49" s="29"/>
-      <c r="ER49" s="29"/>
+      <c r="EQ49" s="28"/>
+      <c r="ER49" s="28"/>
       <c r="ES49" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -4456,28 +4456,28 @@
       <c r="EA50" s="22">
         <v>6</v>
       </c>
-      <c r="EB50" s="29" t="s">
+      <c r="EB50" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="EC50" s="29"/>
-      <c r="ED50" s="29"/>
-      <c r="EE50" s="29"/>
-      <c r="EF50" s="29"/>
-      <c r="EM50" s="28">
+      <c r="EC50" s="28"/>
+      <c r="ED50" s="28"/>
+      <c r="EE50" s="28"/>
+      <c r="EF50" s="28"/>
+      <c r="EM50" s="29">
         <v>9</v>
       </c>
-      <c r="EN50" s="29"/>
-      <c r="EO50" s="29"/>
-      <c r="EP50" s="28">
+      <c r="EN50" s="28"/>
+      <c r="EO50" s="28"/>
+      <c r="EP50" s="29">
         <v>22</v>
       </c>
-      <c r="EQ50" s="29"/>
-      <c r="ER50" s="29"/>
+      <c r="EQ50" s="28"/>
+      <c r="ER50" s="28"/>
       <c r="ES50" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -4654,28 +4654,28 @@
       <c r="EA51" s="21">
         <v>7</v>
       </c>
-      <c r="EB51" s="29" t="s">
+      <c r="EB51" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="EC51" s="29"/>
-      <c r="ED51" s="29"/>
-      <c r="EE51" s="29"/>
-      <c r="EF51" s="29"/>
-      <c r="EM51" s="28">
+      <c r="EC51" s="28"/>
+      <c r="ED51" s="28"/>
+      <c r="EE51" s="28"/>
+      <c r="EF51" s="28"/>
+      <c r="EM51" s="29">
         <v>19</v>
       </c>
-      <c r="EN51" s="29"/>
-      <c r="EO51" s="29"/>
-      <c r="EP51" s="28">
-        <v>0</v>
-      </c>
-      <c r="EQ51" s="29"/>
-      <c r="ER51" s="29"/>
+      <c r="EN51" s="28"/>
+      <c r="EO51" s="28"/>
+      <c r="EP51" s="29">
+        <v>0</v>
+      </c>
+      <c r="EQ51" s="28"/>
+      <c r="ER51" s="28"/>
       <c r="ES51" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -4852,28 +4852,28 @@
       <c r="EA52" s="16">
         <v>8</v>
       </c>
-      <c r="EB52" s="29" t="s">
+      <c r="EB52" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="EC52" s="29"/>
-      <c r="ED52" s="29"/>
-      <c r="EE52" s="29"/>
-      <c r="EF52" s="29"/>
-      <c r="EM52" s="28">
+      <c r="EC52" s="28"/>
+      <c r="ED52" s="28"/>
+      <c r="EE52" s="28"/>
+      <c r="EF52" s="28"/>
+      <c r="EM52" s="29">
         <v>25</v>
       </c>
-      <c r="EN52" s="29"/>
-      <c r="EO52" s="29"/>
-      <c r="EP52" s="28">
+      <c r="EN52" s="28"/>
+      <c r="EO52" s="28"/>
+      <c r="EP52" s="29">
         <v>7</v>
       </c>
-      <c r="EQ52" s="29"/>
-      <c r="ER52" s="29"/>
+      <c r="EQ52" s="28"/>
+      <c r="ER52" s="28"/>
       <c r="ES52" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -5057,28 +5057,28 @@
       <c r="EA53" s="20">
         <v>9</v>
       </c>
-      <c r="EB53" s="29" t="s">
+      <c r="EB53" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="EC53" s="29"/>
-      <c r="ED53" s="29"/>
-      <c r="EE53" s="29"/>
-      <c r="EF53" s="29"/>
-      <c r="EM53" s="28">
+      <c r="EC53" s="28"/>
+      <c r="ED53" s="28"/>
+      <c r="EE53" s="28"/>
+      <c r="EF53" s="28"/>
+      <c r="EM53" s="29">
         <v>37</v>
       </c>
-      <c r="EN53" s="29"/>
-      <c r="EO53" s="29"/>
-      <c r="EP53" s="28">
+      <c r="EN53" s="28"/>
+      <c r="EO53" s="28"/>
+      <c r="EP53" s="29">
         <v>24</v>
       </c>
-      <c r="EQ53" s="29"/>
-      <c r="ER53" s="29"/>
+      <c r="EQ53" s="28"/>
+      <c r="ER53" s="28"/>
       <c r="ES53" s="23">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -5263,28 +5263,28 @@
       <c r="EA54" s="15">
         <v>10</v>
       </c>
-      <c r="EB54" s="29" t="s">
+      <c r="EB54" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="EC54" s="29"/>
-      <c r="ED54" s="29"/>
-      <c r="EE54" s="29"/>
-      <c r="EF54" s="29"/>
-      <c r="EM54" s="28">
+      <c r="EC54" s="28"/>
+      <c r="ED54" s="28"/>
+      <c r="EE54" s="28"/>
+      <c r="EF54" s="28"/>
+      <c r="EM54" s="29">
         <v>32</v>
       </c>
-      <c r="EN54" s="29"/>
-      <c r="EO54" s="29"/>
-      <c r="EP54" s="28">
+      <c r="EN54" s="28"/>
+      <c r="EO54" s="28"/>
+      <c r="EP54" s="29">
         <v>16</v>
       </c>
-      <c r="EQ54" s="29"/>
-      <c r="ER54" s="29"/>
+      <c r="EQ54" s="28"/>
+      <c r="ER54" s="28"/>
       <c r="ES54" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -5466,28 +5466,28 @@
       <c r="EA55" s="19">
         <v>11</v>
       </c>
-      <c r="EB55" s="29" t="s">
+      <c r="EB55" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="EC55" s="29"/>
-      <c r="ED55" s="29"/>
-      <c r="EE55" s="29"/>
-      <c r="EF55" s="29"/>
-      <c r="EM55" s="28">
+      <c r="EC55" s="28"/>
+      <c r="ED55" s="28"/>
+      <c r="EE55" s="28"/>
+      <c r="EF55" s="28"/>
+      <c r="EM55" s="29">
         <v>18</v>
       </c>
-      <c r="EN55" s="29"/>
-      <c r="EO55" s="29"/>
-      <c r="EP55" s="28">
+      <c r="EN55" s="28"/>
+      <c r="EO55" s="28"/>
+      <c r="EP55" s="29">
         <v>24</v>
       </c>
-      <c r="EQ55" s="29"/>
-      <c r="ER55" s="29"/>
+      <c r="EQ55" s="28"/>
+      <c r="ER55" s="28"/>
       <c r="ES55" s="23">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -5674,21 +5674,21 @@
       <c r="EA56" s="14">
         <v>12</v>
       </c>
-      <c r="EB56" s="29" t="s">
+      <c r="EB56" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="EC56" s="29"/>
-      <c r="ED56" s="29"/>
-      <c r="EE56" s="29"/>
-      <c r="EF56" s="29"/>
-      <c r="EM56" s="28"/>
-      <c r="EN56" s="29"/>
-      <c r="EO56" s="29"/>
-      <c r="EP56" s="28"/>
-      <c r="EQ56" s="29"/>
-      <c r="ER56" s="29"/>
+      <c r="EC56" s="28"/>
+      <c r="ED56" s="28"/>
+      <c r="EE56" s="28"/>
+      <c r="EF56" s="28"/>
+      <c r="EM56" s="29"/>
+      <c r="EN56" s="28"/>
+      <c r="EO56" s="28"/>
+      <c r="EP56" s="29"/>
+      <c r="EQ56" s="28"/>
+      <c r="ER56" s="28"/>
     </row>
-    <row r="57" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -5865,24 +5865,24 @@
       <c r="EA57" s="18">
         <v>13</v>
       </c>
-      <c r="EB57" s="29" t="s">
+      <c r="EB57" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="EC57" s="29"/>
-      <c r="ED57" s="29"/>
-      <c r="EE57" s="29"/>
-      <c r="EF57" s="29"/>
-      <c r="EG57" s="29"/>
-      <c r="EH57" s="29"/>
-      <c r="EI57" s="29"/>
-      <c r="EM57" s="28"/>
-      <c r="EN57" s="29"/>
-      <c r="EO57" s="29"/>
-      <c r="EP57" s="28"/>
-      <c r="EQ57" s="29"/>
-      <c r="ER57" s="29"/>
+      <c r="EC57" s="28"/>
+      <c r="ED57" s="28"/>
+      <c r="EE57" s="28"/>
+      <c r="EF57" s="28"/>
+      <c r="EG57" s="28"/>
+      <c r="EH57" s="28"/>
+      <c r="EI57" s="28"/>
+      <c r="EM57" s="29"/>
+      <c r="EN57" s="28"/>
+      <c r="EO57" s="28"/>
+      <c r="EP57" s="29"/>
+      <c r="EQ57" s="28"/>
+      <c r="ER57" s="28"/>
     </row>
-    <row r="58" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -6037,13 +6037,13 @@
       <c r="EA58" s="18">
         <v>16</v>
       </c>
-      <c r="EB58" s="29" t="s">
+      <c r="EB58" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="EC58" s="29"/>
-      <c r="ED58" s="29"/>
-      <c r="EE58" s="29"/>
-      <c r="EF58" s="29"/>
+      <c r="EC58" s="28"/>
+      <c r="ED58" s="28"/>
+      <c r="EE58" s="28"/>
+      <c r="EF58" s="28"/>
       <c r="EM58" s="24"/>
       <c r="EN58" s="25"/>
       <c r="EO58" s="25"/>
@@ -6051,7 +6051,7 @@
       <c r="EQ58" s="25"/>
       <c r="ER58" s="25"/>
     </row>
-    <row r="59" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -6205,16 +6205,16 @@
       <c r="EA59" s="18">
         <v>17</v>
       </c>
-      <c r="EB59" s="29" t="s">
+      <c r="EB59" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="EC59" s="29"/>
-      <c r="ED59" s="29"/>
-      <c r="EE59" s="29"/>
-      <c r="EF59" s="29"/>
-      <c r="EG59" s="29"/>
-      <c r="EH59" s="29"/>
-      <c r="EI59" s="29"/>
+      <c r="EC59" s="28"/>
+      <c r="ED59" s="28"/>
+      <c r="EE59" s="28"/>
+      <c r="EF59" s="28"/>
+      <c r="EG59" s="28"/>
+      <c r="EH59" s="28"/>
+      <c r="EI59" s="28"/>
       <c r="EM59" s="24"/>
       <c r="EN59" s="25"/>
       <c r="EO59" s="25"/>
@@ -6222,7 +6222,7 @@
       <c r="EQ59" s="25"/>
       <c r="ER59" s="25"/>
     </row>
-    <row r="60" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -6380,7 +6380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -6559,7 +6559,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -6730,15 +6730,15 @@
       <c r="EA62" s="15">
         <v>14</v>
       </c>
-      <c r="EB62" s="29" t="s">
+      <c r="EB62" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="EC62" s="29"/>
-      <c r="ED62" s="29"/>
-      <c r="EE62" s="29"/>
-      <c r="EF62" s="29"/>
+      <c r="EC62" s="28"/>
+      <c r="ED62" s="28"/>
+      <c r="EE62" s="28"/>
+      <c r="EF62" s="28"/>
     </row>
-    <row r="63" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -6898,19 +6898,19 @@
       <c r="EA63" s="15">
         <v>15</v>
       </c>
-      <c r="EB63" s="29" t="s">
+      <c r="EB63" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="EC63" s="29"/>
-      <c r="ED63" s="29"/>
-      <c r="EE63" s="29"/>
-      <c r="EF63" s="29"/>
-      <c r="EG63" s="29"/>
-      <c r="EH63" s="29"/>
-      <c r="EI63" s="29"/>
-      <c r="EJ63" s="29"/>
+      <c r="EC63" s="28"/>
+      <c r="ED63" s="28"/>
+      <c r="EE63" s="28"/>
+      <c r="EF63" s="28"/>
+      <c r="EG63" s="28"/>
+      <c r="EH63" s="28"/>
+      <c r="EI63" s="28"/>
+      <c r="EJ63" s="28"/>
     </row>
-    <row r="64" spans="2:149" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:149" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -7066,7 +7066,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -7216,7 +7216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -7251,7 +7251,7 @@
       <c r="BS66" s="4"/>
       <c r="BT66" s="4"/>
     </row>
-    <row r="67" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -7273,7 +7273,7 @@
       <c r="BS67" s="4"/>
       <c r="BT67" s="4"/>
     </row>
-    <row r="68" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -7304,7 +7304,7 @@
       <c r="BS68" s="4"/>
       <c r="BT68" s="4"/>
     </row>
-    <row r="69" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -7345,7 +7345,7 @@
       <c r="BS69" s="4"/>
       <c r="BT69" s="4"/>
     </row>
-    <row r="70" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -7371,7 +7371,7 @@
       <c r="BS70" s="4"/>
       <c r="BT70" s="4"/>
     </row>
-    <row r="71" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
@@ -7414,8 +7414,77 @@
       <c r="BR71" s="4"/>
       <c r="BS71" s="4"/>
       <c r="BT71" s="4"/>
+      <c r="CE71" s="12">
+        <v>0</v>
+      </c>
+      <c r="CF71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CH71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CI71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CJ71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CK71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CL71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CM71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CN71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CO71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CP71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CQ71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CR71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CS71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CT71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CU71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CV71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CW71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CX71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CY71" s="13">
+        <v>3</v>
+      </c>
+      <c r="CZ71" s="13">
+        <v>3</v>
+      </c>
+      <c r="DA71" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="72" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="R72" s="4"/>
@@ -7442,8 +7511,77 @@
       <c r="BR72" s="4"/>
       <c r="BS72" s="4"/>
       <c r="BT72" s="4"/>
+      <c r="CE72" s="12">
+        <v>1</v>
+      </c>
+      <c r="CF72" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY72" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ72" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA72" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="73" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="E73" s="10"/>
@@ -7478,8 +7616,77 @@
       <c r="BR73" s="4"/>
       <c r="BS73" s="4"/>
       <c r="BT73" s="4"/>
+      <c r="CE73" s="12">
+        <v>2</v>
+      </c>
+      <c r="CF73" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI73" s="14">
+        <v>12</v>
+      </c>
+      <c r="CJ73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY73" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ73" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA73" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="74" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="R74" s="4"/>
@@ -7506,8 +7713,77 @@
       <c r="BR74" s="4"/>
       <c r="BS74" s="4"/>
       <c r="BT74" s="4"/>
+      <c r="CE74" s="12">
+        <v>3</v>
+      </c>
+      <c r="CF74" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI74" s="14">
+        <v>12</v>
+      </c>
+      <c r="CJ74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX74" s="14">
+        <v>12</v>
+      </c>
+      <c r="CY74" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ74" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA74" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="75" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -7560,8 +7836,77 @@
       <c r="BR75" s="4"/>
       <c r="BS75" s="4"/>
       <c r="BT75" s="4"/>
+      <c r="CE75" s="12">
+        <v>4</v>
+      </c>
+      <c r="CF75" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI75" s="14">
+        <v>12</v>
+      </c>
+      <c r="CJ75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO75" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP75" s="14">
+        <v>12</v>
+      </c>
+      <c r="CQ75" s="14">
+        <v>12</v>
+      </c>
+      <c r="CR75" s="14">
+        <v>12</v>
+      </c>
+      <c r="CS75" s="14">
+        <v>12</v>
+      </c>
+      <c r="CT75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY75" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ75" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA75" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="76" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -7615,8 +7960,77 @@
       <c r="BR76" s="4"/>
       <c r="BS76" s="4"/>
       <c r="BT76" s="4"/>
+      <c r="CE76" s="12">
+        <v>5</v>
+      </c>
+      <c r="CF76" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI76" s="14">
+        <v>12</v>
+      </c>
+      <c r="CJ76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY76" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ76" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA76" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="77" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -7688,8 +8102,148 @@
       <c r="BR77" s="4"/>
       <c r="BS77" s="4"/>
       <c r="BT77" s="4"/>
+      <c r="CE77" s="12">
+        <v>6</v>
+      </c>
+      <c r="CF77" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI77" s="14">
+        <v>12</v>
+      </c>
+      <c r="CJ77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW77" s="14">
+        <v>12</v>
+      </c>
+      <c r="CX77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY77" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ77" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA77" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="79" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CE78" s="12">
+        <v>7</v>
+      </c>
+      <c r="CF78" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY78" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ78" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA78" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="13">
         <v>3</v>
       </c>
@@ -7903,8 +8457,77 @@
       <c r="BT79" s="13">
         <v>3</v>
       </c>
+      <c r="CE79" s="12">
+        <v>8</v>
+      </c>
+      <c r="CF79" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL79" s="14">
+        <v>12</v>
+      </c>
+      <c r="CM79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO79" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY79" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ79" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA79" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="80" spans="2:126" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="13">
         <v>3</v>
       </c>
@@ -8118,8 +8741,77 @@
       <c r="BT80" s="13">
         <v>3</v>
       </c>
+      <c r="CE80" s="12">
+        <v>9</v>
+      </c>
+      <c r="CF80" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO80" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU80" s="14">
+        <v>12</v>
+      </c>
+      <c r="CV80" s="14">
+        <v>12</v>
+      </c>
+      <c r="CW80" s="14">
+        <v>12</v>
+      </c>
+      <c r="CX80" s="14">
+        <v>12</v>
+      </c>
+      <c r="CY80" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ80" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA80" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="81" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="13">
         <v>3</v>
       </c>
@@ -8333,8 +9025,77 @@
       <c r="BT81" s="13">
         <v>3</v>
       </c>
+      <c r="CE81" s="12">
+        <v>10</v>
+      </c>
+      <c r="CF81" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ81" s="14">
+        <v>12</v>
+      </c>
+      <c r="CK81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO81" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU81" s="14">
+        <v>12</v>
+      </c>
+      <c r="CV81" s="14">
+        <v>12</v>
+      </c>
+      <c r="CW81" s="14">
+        <v>12</v>
+      </c>
+      <c r="CX81" s="14">
+        <v>12</v>
+      </c>
+      <c r="CY81" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ81" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA81" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="82" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="13">
         <v>3</v>
       </c>
@@ -8548,8 +9309,77 @@
       <c r="BT82" s="13">
         <v>3</v>
       </c>
+      <c r="CE82" s="12">
+        <v>11</v>
+      </c>
+      <c r="CF82" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO82" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU82" s="14">
+        <v>12</v>
+      </c>
+      <c r="CV82" s="14">
+        <v>12</v>
+      </c>
+      <c r="CW82" s="14">
+        <v>12</v>
+      </c>
+      <c r="CX82" s="14">
+        <v>12</v>
+      </c>
+      <c r="CY82" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ82" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA82" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="83" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="13">
         <v>3</v>
       </c>
@@ -8763,8 +9593,77 @@
       <c r="BT83" s="13">
         <v>3</v>
       </c>
+      <c r="CE83" s="12">
+        <v>12</v>
+      </c>
+      <c r="CF83" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL83" s="14">
+        <v>12</v>
+      </c>
+      <c r="CM83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO83" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU83" s="14">
+        <v>12</v>
+      </c>
+      <c r="CV83" s="14">
+        <v>12</v>
+      </c>
+      <c r="CW83" s="14">
+        <v>12</v>
+      </c>
+      <c r="CX83" s="14">
+        <v>12</v>
+      </c>
+      <c r="CY83" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ83" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA83" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="84" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="13">
         <v>3</v>
       </c>
@@ -8978,8 +9877,77 @@
       <c r="BT84" s="13">
         <v>3</v>
       </c>
+      <c r="CE84" s="12">
+        <v>13</v>
+      </c>
+      <c r="CF84" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO84" s="14">
+        <v>12</v>
+      </c>
+      <c r="CP84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY84" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ84" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA84" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="85" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="13">
         <v>3</v>
       </c>
@@ -9193,8 +10161,77 @@
       <c r="BT85" s="13">
         <v>3</v>
       </c>
+      <c r="CE85" s="12">
+        <v>14</v>
+      </c>
+      <c r="CF85" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CH85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CI85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CJ85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CK85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CL85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CM85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CN85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CO85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CP85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CQ85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CR85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CS85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CT85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CU85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CV85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CW85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CX85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CY85" s="17">
+        <v>0</v>
+      </c>
+      <c r="CZ85" s="17">
+        <v>0</v>
+      </c>
+      <c r="DA85" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="86" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="13">
         <v>3</v>
       </c>
@@ -9408,8 +10445,77 @@
       <c r="BT86" s="13">
         <v>3</v>
       </c>
+      <c r="CE86" s="12">
+        <v>15</v>
+      </c>
+      <c r="CF86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CG86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CH86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CI86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CJ86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CK86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CL86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CM86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CN86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CO86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CP86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CQ86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CR86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CS86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CT86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CU86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CV86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CW86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CX86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CY86" s="13">
+        <v>3</v>
+      </c>
+      <c r="CZ86" s="13">
+        <v>3</v>
+      </c>
+      <c r="DA86" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="87" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="13">
         <v>3</v>
       </c>
@@ -9623,8 +10729,74 @@
       <c r="BT87" s="13">
         <v>3</v>
       </c>
+      <c r="CF87" s="12">
+        <v>0</v>
+      </c>
+      <c r="CG87" s="12">
+        <v>1</v>
+      </c>
+      <c r="CH87" s="12">
+        <v>2</v>
+      </c>
+      <c r="CI87" s="12">
+        <v>3</v>
+      </c>
+      <c r="CJ87" s="12">
+        <v>4</v>
+      </c>
+      <c r="CK87" s="12">
+        <v>5</v>
+      </c>
+      <c r="CL87" s="12">
+        <v>6</v>
+      </c>
+      <c r="CM87" s="12">
+        <v>7</v>
+      </c>
+      <c r="CN87" s="12">
+        <v>8</v>
+      </c>
+      <c r="CO87" s="12">
+        <v>9</v>
+      </c>
+      <c r="CP87" s="12">
+        <v>10</v>
+      </c>
+      <c r="CQ87" s="12">
+        <v>11</v>
+      </c>
+      <c r="CR87" s="12">
+        <v>12</v>
+      </c>
+      <c r="CS87" s="12">
+        <v>13</v>
+      </c>
+      <c r="CT87" s="12">
+        <v>14</v>
+      </c>
+      <c r="CU87" s="12">
+        <v>15</v>
+      </c>
+      <c r="CV87" s="12">
+        <v>16</v>
+      </c>
+      <c r="CW87" s="12">
+        <v>17</v>
+      </c>
+      <c r="CX87" s="12">
+        <v>18</v>
+      </c>
+      <c r="CY87" s="12">
+        <v>19</v>
+      </c>
+      <c r="CZ87" s="12">
+        <v>20</v>
+      </c>
+      <c r="DA87" s="12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="88" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="13">
         <v>3</v>
       </c>
@@ -9839,7 +11011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="13">
         <v>3</v>
       </c>
@@ -10054,7 +11226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="13">
         <v>3</v>
       </c>
@@ -10269,7 +11441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="13">
         <v>3</v>
       </c>
@@ -10484,7 +11656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="13">
         <v>3</v>
       </c>
@@ -10699,7 +11871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="13">
         <v>3</v>
       </c>
@@ -10914,7 +12086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="13">
         <v>3</v>
       </c>
@@ -11129,7 +12301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="13">
         <v>3</v>
       </c>
@@ -11344,7 +12516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:105" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="13">
         <v>3</v>
       </c>
@@ -11559,7 +12731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="13">
         <v>3</v>
       </c>
@@ -11774,7 +12946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="13">
         <v>3</v>
       </c>
@@ -11989,7 +13161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="13">
         <v>3</v>
       </c>
@@ -12204,7 +13376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="13">
         <v>3</v>
       </c>
@@ -12419,7 +13591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="13">
         <v>3</v>
       </c>
@@ -12634,7 +13806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="13">
         <v>3</v>
       </c>
@@ -12849,7 +14021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="13">
         <v>3</v>
       </c>
@@ -13064,7 +14236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="13">
         <v>3</v>
       </c>
@@ -13279,7 +14451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="13">
         <v>3</v>
       </c>
@@ -13494,7 +14666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="13">
         <v>3</v>
       </c>
@@ -13709,7 +14881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="13">
         <v>3</v>
       </c>
@@ -13924,7 +15096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="13">
         <v>3</v>
       </c>
@@ -14139,7 +15311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="13">
         <v>3</v>
       </c>
@@ -14354,7 +15526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="13">
         <v>3</v>
       </c>
@@ -14569,7 +15741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="13">
         <v>3</v>
       </c>
@@ -14784,7 +15956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="13">
         <v>3</v>
       </c>
@@ -14999,7 +16171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="13">
         <v>3</v>
       </c>
@@ -15214,7 +16386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="13">
         <v>3</v>
       </c>
@@ -15429,7 +16601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="13">
         <v>3</v>
       </c>
@@ -15644,138 +16816,138 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC120" s="23">
         <v>0</v>
       </c>
-      <c r="AD120" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE120" s="28"/>
-      <c r="AF120" s="28"/>
-      <c r="AG120" s="28"/>
-      <c r="AH120" s="28"/>
+      <c r="AD120" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE120" s="29"/>
+      <c r="AF120" s="29"/>
+      <c r="AG120" s="29"/>
+      <c r="AH120" s="29"/>
     </row>
-    <row r="121" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC121" s="23">
         <v>1</v>
       </c>
-      <c r="AD121" s="28" t="s">
+      <c r="AD121" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="AE121" s="28"/>
-      <c r="AF121" s="28"/>
-      <c r="AG121" s="28"/>
-      <c r="AH121" s="28"/>
+      <c r="AE121" s="29"/>
+      <c r="AF121" s="29"/>
+      <c r="AG121" s="29"/>
+      <c r="AH121" s="29"/>
     </row>
-    <row r="122" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC122" s="23">
         <v>2</v>
       </c>
-      <c r="AD122" s="28" t="s">
+      <c r="AD122" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="AE122" s="28"/>
-      <c r="AF122" s="28"/>
-      <c r="AG122" s="28"/>
-      <c r="AH122" s="28"/>
+      <c r="AE122" s="29"/>
+      <c r="AF122" s="29"/>
+      <c r="AG122" s="29"/>
+      <c r="AH122" s="29"/>
     </row>
-    <row r="123" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC123" s="23">
         <v>3</v>
       </c>
-      <c r="AD123" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE123" s="28"/>
-      <c r="AF123" s="28"/>
-      <c r="AG123" s="28"/>
-      <c r="AH123" s="28"/>
+      <c r="AD123" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE123" s="29"/>
+      <c r="AF123" s="29"/>
+      <c r="AG123" s="29"/>
+      <c r="AH123" s="29"/>
     </row>
-    <row r="124" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC124" s="23">
         <v>4</v>
       </c>
-      <c r="AD124" s="28" t="s">
+      <c r="AD124" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AE124" s="28"/>
-      <c r="AF124" s="28"/>
-      <c r="AG124" s="28"/>
-      <c r="AH124" s="28"/>
+      <c r="AE124" s="29"/>
+      <c r="AF124" s="29"/>
+      <c r="AG124" s="29"/>
+      <c r="AH124" s="29"/>
     </row>
-    <row r="125" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC125" s="23">
         <v>5</v>
       </c>
-      <c r="AD125" s="28" t="s">
+      <c r="AD125" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="AE125" s="28"/>
-      <c r="AF125" s="28"/>
-      <c r="AG125" s="28"/>
-      <c r="AH125" s="28"/>
+      <c r="AE125" s="29"/>
+      <c r="AF125" s="29"/>
+      <c r="AG125" s="29"/>
+      <c r="AH125" s="29"/>
     </row>
-    <row r="126" spans="2:72" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:72" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC126" s="23">
         <v>6</v>
       </c>
-      <c r="AD126" s="28" t="s">
+      <c r="AD126" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="AE126" s="28"/>
-      <c r="AF126" s="28"/>
-      <c r="AG126" s="28"/>
-      <c r="AH126" s="28"/>
+      <c r="AE126" s="29"/>
+      <c r="AF126" s="29"/>
+      <c r="AG126" s="29"/>
+      <c r="AH126" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="EB44:EF44"/>
-    <mergeCell ref="EB45:EF45"/>
-    <mergeCell ref="EB46:EF46"/>
-    <mergeCell ref="EB47:EF47"/>
-    <mergeCell ref="EM47:ER47"/>
+    <mergeCell ref="AD126:AH126"/>
+    <mergeCell ref="AD121:AH121"/>
+    <mergeCell ref="AD122:AH122"/>
+    <mergeCell ref="AD123:AH123"/>
+    <mergeCell ref="AD124:AH124"/>
+    <mergeCell ref="AD125:AH125"/>
+    <mergeCell ref="EB58:EF58"/>
+    <mergeCell ref="EB59:EI59"/>
+    <mergeCell ref="EB62:EF62"/>
+    <mergeCell ref="EB63:EJ63"/>
+    <mergeCell ref="AD120:AH120"/>
+    <mergeCell ref="EB56:EF56"/>
+    <mergeCell ref="EM56:EO56"/>
+    <mergeCell ref="EP56:ER56"/>
+    <mergeCell ref="EB57:EI57"/>
+    <mergeCell ref="EM57:EO57"/>
+    <mergeCell ref="EP57:ER57"/>
+    <mergeCell ref="EB54:EF54"/>
+    <mergeCell ref="EM54:EO54"/>
+    <mergeCell ref="EP54:ER54"/>
+    <mergeCell ref="EB55:EF55"/>
+    <mergeCell ref="EM55:EO55"/>
+    <mergeCell ref="EP55:ER55"/>
+    <mergeCell ref="EB52:EF52"/>
+    <mergeCell ref="EM52:EO52"/>
+    <mergeCell ref="EP52:ER52"/>
+    <mergeCell ref="EB53:EF53"/>
+    <mergeCell ref="EM53:EO53"/>
+    <mergeCell ref="EP53:ER53"/>
+    <mergeCell ref="EB50:EF50"/>
+    <mergeCell ref="EM50:EO50"/>
+    <mergeCell ref="EP50:ER50"/>
+    <mergeCell ref="EB51:EF51"/>
+    <mergeCell ref="EM51:EO51"/>
+    <mergeCell ref="EP51:ER51"/>
     <mergeCell ref="EB48:EF48"/>
     <mergeCell ref="EM48:EO48"/>
     <mergeCell ref="EP48:ER48"/>
     <mergeCell ref="EB49:EF49"/>
     <mergeCell ref="EM49:EO49"/>
     <mergeCell ref="EP49:ER49"/>
-    <mergeCell ref="EB50:EF50"/>
-    <mergeCell ref="EM50:EO50"/>
-    <mergeCell ref="EP50:ER50"/>
-    <mergeCell ref="EB51:EF51"/>
-    <mergeCell ref="EM51:EO51"/>
-    <mergeCell ref="EP51:ER51"/>
-    <mergeCell ref="EB52:EF52"/>
-    <mergeCell ref="EM52:EO52"/>
-    <mergeCell ref="EP52:ER52"/>
-    <mergeCell ref="EB53:EF53"/>
-    <mergeCell ref="EM53:EO53"/>
-    <mergeCell ref="EP53:ER53"/>
-    <mergeCell ref="EB54:EF54"/>
-    <mergeCell ref="EM54:EO54"/>
-    <mergeCell ref="EP54:ER54"/>
-    <mergeCell ref="EB55:EF55"/>
-    <mergeCell ref="EM55:EO55"/>
-    <mergeCell ref="EP55:ER55"/>
-    <mergeCell ref="EB56:EF56"/>
-    <mergeCell ref="EM56:EO56"/>
-    <mergeCell ref="EP56:ER56"/>
-    <mergeCell ref="EB57:EI57"/>
-    <mergeCell ref="EM57:EO57"/>
-    <mergeCell ref="EP57:ER57"/>
-    <mergeCell ref="EB58:EF58"/>
-    <mergeCell ref="EB59:EI59"/>
-    <mergeCell ref="EB62:EF62"/>
-    <mergeCell ref="EB63:EJ63"/>
-    <mergeCell ref="AD120:AH120"/>
-    <mergeCell ref="AD126:AH126"/>
-    <mergeCell ref="AD121:AH121"/>
-    <mergeCell ref="AD122:AH122"/>
-    <mergeCell ref="AD123:AH123"/>
-    <mergeCell ref="AD124:AH124"/>
-    <mergeCell ref="AD125:AH125"/>
+    <mergeCell ref="EB44:EF44"/>
+    <mergeCell ref="EB45:EF45"/>
+    <mergeCell ref="EB46:EF46"/>
+    <mergeCell ref="EB47:EF47"/>
+    <mergeCell ref="EM47:ER47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>